<commit_message>
Subo Foleys y tabla metadatos
Subo algunos Foleys y la tabla con los datos completados de los sonidos Foley
</commit_message>
<xml_diff>
--- a/Tablas de sonido/Tabla_metadatos_no_lineal.xlsx
+++ b/Tablas de sonido/Tabla_metadatos_no_lineal.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="309">
   <si>
     <t>Tabla de metadatos - Música</t>
   </si>
@@ -305,34 +305,16 @@
     <t>SFX/Personaje flamenca taconeo/sonido1</t>
   </si>
   <si>
-    <t>https://drive.google.com/drive/folders/1UnFbVGLqAOiS5xas9gw_-94HSp7m-Q0Q?usp=sharing</t>
-  </si>
-  <si>
     <t>22.5 kHz</t>
   </si>
   <si>
     <t>SFX/Arma flauta/sonido1</t>
   </si>
   <si>
-    <t>https://drive.google.com/drive/folders/12HrWDrHcXC6v38MHVuomd5-b7fe3dz-C?usp=sharing</t>
-  </si>
-  <si>
     <t>SFX/vendedor/sonido 1</t>
   </si>
   <si>
-    <t>sonido flauta estaba en voces, sonido que tambien esta en ataque flauta (el de arriba pero este sera distinto)</t>
-  </si>
-  <si>
-    <t>SFX/Personaje utiliza castañuelas/sonido de castañuelas</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/drive/folders/1EOg0Ej885RwWcIxBl_yaov9mmHb7b31a?usp=sharing</t>
-  </si>
-  <si>
     <t>SFX/Movimiento bloques/sonido 1</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/drive/folders/105A8VLE-a_QD9Z63zjaMozKcWCt-vNeU?usp=sharing</t>
   </si>
   <si>
     <t>SFX/Personaje Cae al suelo/golpe caida</t>
@@ -342,9 +324,6 @@
   </si>
   <si>
     <t>SFX/Personaje Pasos sobre madera/madera sonido1</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/drive/folders/1f7G1jQis_DXGfJz3qFtkaJV98KX5w_Zy?usp=sharing</t>
   </si>
   <si>
     <t>SFX/Personaje Pasos sobre charcos/charcos sonido1</t>
@@ -772,6 +751,207 @@
   <si>
     <t>Audacity, Sonido grabado, con la frecuencia de muestreo modificada, normalizado a -7,86 db de amplitud</t>
   </si>
+  <si>
+    <t>SFX/Personaje flamenca taconeo/sonido4</t>
+  </si>
+  <si>
+    <t>SFX/Personaje flamenca taconeo/sonido2</t>
+  </si>
+  <si>
+    <t>SFX/Personaje flamenca taconeo/sonido3</t>
+  </si>
+  <si>
+    <t>00:00:95</t>
+  </si>
+  <si>
+    <t>-8,416 db</t>
+  </si>
+  <si>
+    <t>-7,638 db</t>
+  </si>
+  <si>
+    <t>00:03:96</t>
+  </si>
+  <si>
+    <t>-20,022 db</t>
+  </si>
+  <si>
+    <t>00:10:47</t>
+  </si>
+  <si>
+    <t>-17,544db</t>
+  </si>
+  <si>
+    <t>SFX/Arma flauta/sonido2</t>
+  </si>
+  <si>
+    <t>00:01:65</t>
+  </si>
+  <si>
+    <t>-24,586db</t>
+  </si>
+  <si>
+    <t>00:00:93</t>
+  </si>
+  <si>
+    <t>-17,887db</t>
+  </si>
+  <si>
+    <t>SFX/vendedor/sonido 2</t>
+  </si>
+  <si>
+    <t>SFX/vendedor/sonido 3</t>
+  </si>
+  <si>
+    <t>SFX/vendedor/sonido 4</t>
+  </si>
+  <si>
+    <t>SFX/vendedor/sonido 5</t>
+  </si>
+  <si>
+    <t>00:07:12</t>
+  </si>
+  <si>
+    <t>-13,243db</t>
+  </si>
+  <si>
+    <t>00:03:38</t>
+  </si>
+  <si>
+    <t>-12,454db</t>
+  </si>
+  <si>
+    <t>00:11:11</t>
+  </si>
+  <si>
+    <t>-13,495db</t>
+  </si>
+  <si>
+    <t>-7,185db</t>
+  </si>
+  <si>
+    <t>00:05:80</t>
+  </si>
+  <si>
+    <t>-4,796db</t>
+  </si>
+  <si>
+    <t>SFX/Personaje utiliza castañuelas/sonido de castañuelas 1</t>
+  </si>
+  <si>
+    <t>SFX/Personaje utiliza castañuelas/sonido de castañuelas 2</t>
+  </si>
+  <si>
+    <t>00:02:56</t>
+  </si>
+  <si>
+    <t>-11,232db</t>
+  </si>
+  <si>
+    <t>00:11:33</t>
+  </si>
+  <si>
+    <t>-11,173db</t>
+  </si>
+  <si>
+    <t>SFX/Movimiento bloques/sonido 2</t>
+  </si>
+  <si>
+    <t>SFX/Movimiento bloques/sonido 3</t>
+  </si>
+  <si>
+    <t>SFX/Movimiento bloques/sonido 4</t>
+  </si>
+  <si>
+    <t>SFX/Movimiento bloques/sonido 5</t>
+  </si>
+  <si>
+    <t>SFX/Movimiento bloques/sonido 6</t>
+  </si>
+  <si>
+    <t>SFX/Movimiento bloques/sonido 7</t>
+  </si>
+  <si>
+    <t>00:00:73</t>
+  </si>
+  <si>
+    <t>-28,66db</t>
+  </si>
+  <si>
+    <t>00:00:77</t>
+  </si>
+  <si>
+    <t>-33,547db</t>
+  </si>
+  <si>
+    <t>00:00:41</t>
+  </si>
+  <si>
+    <t>-13,252db</t>
+  </si>
+  <si>
+    <t>00:00:70</t>
+  </si>
+  <si>
+    <t>-20,416db</t>
+  </si>
+  <si>
+    <t>00:00:37</t>
+  </si>
+  <si>
+    <t>-11,214db</t>
+  </si>
+  <si>
+    <t>00:00:39</t>
+  </si>
+  <si>
+    <t>-15,872db</t>
+  </si>
+  <si>
+    <t>00:00:63</t>
+  </si>
+  <si>
+    <t>-26,122db</t>
+  </si>
+  <si>
+    <t>SFX/Personaje Pasos sobre madera/madera sonido2</t>
+  </si>
+  <si>
+    <t>SFX/Personaje Pasos sobre madera/madera sonido3</t>
+  </si>
+  <si>
+    <t>SFX/Personaje Pasos sobre madera/madera sonido4</t>
+  </si>
+  <si>
+    <t>SFX/Personaje Pasos sobre madera/madera sonido5</t>
+  </si>
+  <si>
+    <t>00:01:15</t>
+  </si>
+  <si>
+    <t>-18,307db</t>
+  </si>
+  <si>
+    <t>00:00:57</t>
+  </si>
+  <si>
+    <t>-13,97db</t>
+  </si>
+  <si>
+    <t>-15,658db</t>
+  </si>
+  <si>
+    <t>00:00:80</t>
+  </si>
+  <si>
+    <t>-21,534db</t>
+  </si>
+  <si>
+    <t>00:00:62</t>
+  </si>
+  <si>
+    <t>-23,622db</t>
+  </si>
 </sst>
 </file>
 
@@ -781,7 +961,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="d\.m"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -868,11 +1048,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -946,6 +1121,19 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1224,12 +1412,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1467,12 +1655,6 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="21" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1485,7 +1667,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="21" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1494,7 +1676,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="21" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1527,7 +1709,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1537,19 +1719,19 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="21" fontId="20" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="21" fontId="19" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1575,7 +1757,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="21" fontId="21" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="21" fontId="20" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1598,39 +1780,72 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="27" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -3250,8 +3465,8 @@
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1">
       <c r="A4" s="12"/>
-      <c r="B4" s="139" t="s">
-        <v>203</v>
+      <c r="B4" s="137" t="s">
+        <v>196</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="15"/>
@@ -6644,8 +6859,8 @@
       <c r="L3" s="11"/>
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B4" s="139" t="s">
-        <v>203</v>
+      <c r="B4" s="137" t="s">
+        <v>196</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="15"/>
@@ -12225,8 +12440,8 @@
       <c r="L3" s="11"/>
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B4" s="139" t="s">
-        <v>203</v>
+      <c r="B4" s="137" t="s">
+        <v>196</v>
       </c>
       <c r="C4" s="76"/>
       <c r="D4" s="76"/>
@@ -12266,19 +12481,19 @@
       <c r="J5" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="99">
+      <c r="K5" s="97">
         <v>2.1527777777777778E-3</v>
       </c>
-      <c r="L5" s="100" t="s">
-        <v>136</v>
+      <c r="L5" s="98" t="s">
+        <v>129</v>
       </c>
       <c r="N5" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="13.5" customHeight="1">
       <c r="B6" s="13" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -12300,19 +12515,19 @@
       <c r="J6" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="99">
+      <c r="K6" s="97">
         <v>3.2407407407407406E-4</v>
       </c>
-      <c r="L6" s="100" t="s">
-        <v>138</v>
+      <c r="L6" s="98" t="s">
+        <v>131</v>
       </c>
       <c r="N6" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="13.5" customHeight="1">
       <c r="B7" s="13" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -12334,19 +12549,19 @@
       <c r="J7" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="99">
+      <c r="K7" s="97">
         <v>3.2407407407407406E-4</v>
       </c>
-      <c r="L7" s="100" t="s">
-        <v>140</v>
+      <c r="L7" s="98" t="s">
+        <v>133</v>
       </c>
       <c r="N7" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="13.5" customHeight="1">
       <c r="B8" s="13" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -12368,19 +12583,19 @@
       <c r="J8" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="99">
+      <c r="K8" s="97">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="L8" s="100" t="s">
-        <v>142</v>
+      <c r="L8" s="98" t="s">
+        <v>135</v>
       </c>
       <c r="N8" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="13.5" customHeight="1">
       <c r="B9" s="13" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -12402,19 +12617,19 @@
       <c r="J9" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="K9" s="99">
+      <c r="K9" s="97">
         <v>3.9675925925925927E-2</v>
       </c>
-      <c r="L9" s="101" t="s">
-        <v>144</v>
+      <c r="L9" s="99" t="s">
+        <v>137</v>
       </c>
       <c r="N9" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="13.5" customHeight="1">
       <c r="B10" s="13" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
@@ -12436,19 +12651,19 @@
       <c r="J10" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="99">
+      <c r="K10" s="97">
         <v>4.7453703703703704E-4</v>
       </c>
-      <c r="L10" s="101" t="s">
-        <v>146</v>
+      <c r="L10" s="99" t="s">
+        <v>139</v>
       </c>
       <c r="N10" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1">
       <c r="B11" s="13" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
@@ -12474,15 +12689,15 @@
         <v>8.0439814814814818E-3</v>
       </c>
       <c r="L11" s="72" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="N11" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1">
       <c r="B12" s="13" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -12507,16 +12722,16 @@
       <c r="K12" s="66">
         <v>3.7615740740740739E-3</v>
       </c>
-      <c r="L12" s="101" t="s">
-        <v>150</v>
+      <c r="L12" s="99" t="s">
+        <v>143</v>
       </c>
       <c r="N12" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1">
       <c r="B13" s="13" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -12538,19 +12753,19 @@
       <c r="J13" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="99">
+      <c r="K13" s="97">
         <v>6.8287037037037036E-4</v>
       </c>
-      <c r="L13" s="101" t="s">
-        <v>152</v>
+      <c r="L13" s="99" t="s">
+        <v>145</v>
       </c>
       <c r="N13" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="13.5" customHeight="1">
       <c r="B14" s="13" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C14" s="24"/>
       <c r="D14" s="24"/>
@@ -12572,19 +12787,19 @@
       <c r="J14" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="K14" s="102">
+      <c r="K14" s="100">
         <v>5.3819444444444444E-3</v>
       </c>
-      <c r="L14" s="100" t="s">
-        <v>154</v>
+      <c r="L14" s="98" t="s">
+        <v>147</v>
       </c>
       <c r="N14" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1">
       <c r="B15" s="13" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C15" s="24"/>
       <c r="D15" s="24"/>
@@ -12606,19 +12821,19 @@
       <c r="J15" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="K15" s="102">
+      <c r="K15" s="100">
         <v>6.6666666666666671E-3</v>
       </c>
-      <c r="L15" s="100" t="s">
-        <v>156</v>
+      <c r="L15" s="98" t="s">
+        <v>149</v>
       </c>
       <c r="N15" s="27" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1">
       <c r="B16" s="13" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C16" s="24"/>
       <c r="D16" s="24"/>
@@ -12643,16 +12858,16 @@
       <c r="K16" s="66">
         <v>1.5277777777777779E-3</v>
       </c>
-      <c r="L16" s="100" t="s">
-        <v>159</v>
+      <c r="L16" s="98" t="s">
+        <v>152</v>
       </c>
       <c r="N16" s="27" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="2:14" ht="13.5" customHeight="1">
       <c r="B17" s="13" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
@@ -12677,16 +12892,16 @@
       <c r="K17" s="66">
         <v>1.8865740740740742E-3</v>
       </c>
-      <c r="L17" s="101" t="s">
-        <v>161</v>
+      <c r="L17" s="99" t="s">
+        <v>154</v>
       </c>
       <c r="N17" s="27" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="2:14" ht="13.5" customHeight="1">
       <c r="B18" s="13" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
@@ -12711,16 +12926,16 @@
       <c r="K18" s="66">
         <v>7.5231481481481482E-4</v>
       </c>
-      <c r="L18" s="101" t="s">
-        <v>163</v>
+      <c r="L18" s="99" t="s">
+        <v>156</v>
       </c>
       <c r="N18" s="27" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="2:14" ht="13.5" customHeight="1">
       <c r="B19" s="13" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
@@ -12742,19 +12957,19 @@
       <c r="J19" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="K19" s="102">
+      <c r="K19" s="100">
         <v>1.2037037037037038E-3</v>
       </c>
-      <c r="L19" s="101" t="s">
-        <v>165</v>
+      <c r="L19" s="99" t="s">
+        <v>158</v>
       </c>
       <c r="N19" s="27" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="2:14" ht="13.5" customHeight="1">
       <c r="B20" s="13" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C20" s="24"/>
       <c r="D20" s="24"/>
@@ -12776,19 +12991,19 @@
       <c r="J20" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="K20" s="103">
+      <c r="K20" s="101">
         <v>3.6805555555555554E-3</v>
       </c>
-      <c r="L20" s="101" t="s">
-        <v>167</v>
+      <c r="L20" s="99" t="s">
+        <v>160</v>
       </c>
       <c r="N20" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="2:14" ht="13.5" customHeight="1">
       <c r="B21" s="13" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C21" s="24"/>
       <c r="D21" s="24"/>
@@ -12813,16 +13028,16 @@
       <c r="K21" s="66">
         <v>3.6805555555555554E-3</v>
       </c>
-      <c r="L21" s="101" t="s">
-        <v>167</v>
+      <c r="L21" s="99" t="s">
+        <v>160</v>
       </c>
       <c r="N21" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="2:14" ht="13.5" customHeight="1">
       <c r="B22" s="13" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
@@ -12844,52 +13059,52 @@
       <c r="J22" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="K22" s="103">
+      <c r="K22" s="101">
         <v>5.5439814814814813E-3</v>
       </c>
       <c r="L22" s="72" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="N22" s="27" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="2:14" ht="13.5" customHeight="1">
       <c r="B23" s="30" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C23" s="31"/>
       <c r="D23" s="31"/>
       <c r="E23" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="104" t="s">
+      <c r="F23" s="102" t="s">
         <v>79</v>
       </c>
-      <c r="G23" s="105" t="s">
+      <c r="G23" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="H23" s="106">
+      <c r="H23" s="104">
         <v>16</v>
       </c>
-      <c r="I23" s="106">
+      <c r="I23" s="104">
         <v>32</v>
       </c>
-      <c r="J23" s="105" t="s">
+      <c r="J23" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="K23" s="107">
+      <c r="K23" s="105">
         <v>3.5185185185185185E-3</v>
       </c>
-      <c r="L23" s="108" t="s">
-        <v>172</v>
+      <c r="L23" s="106" t="s">
+        <v>165</v>
       </c>
       <c r="N23" s="27" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B24" s="109"/>
+      <c r="B24" s="107"/>
       <c r="C24" s="38">
         <f t="shared" ref="C24:E24" si="0">COUNTA(C4:C23)</f>
         <v>0</v>
@@ -12904,19 +13119,19 @@
       </c>
     </row>
     <row r="25" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B25" s="109"/>
+      <c r="B25" s="107"/>
       <c r="C25" s="38"/>
       <c r="D25" s="38"/>
       <c r="E25" s="38"/>
     </row>
     <row r="26" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B26" s="109"/>
+      <c r="B26" s="107"/>
       <c r="C26" s="38"/>
       <c r="D26" s="38"/>
       <c r="E26" s="38"/>
     </row>
     <row r="27" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B27" s="109"/>
+      <c r="B27" s="107"/>
       <c r="C27" s="38"/>
       <c r="D27" s="38"/>
       <c r="E27" s="38"/>
@@ -17789,10 +18004,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z1011"/>
+  <dimension ref="A1:Z1030"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -17805,8 +18020,7 @@
     <col min="8" max="8" width="9.7109375" customWidth="1"/>
     <col min="9" max="9" width="15.42578125" customWidth="1"/>
     <col min="10" max="10" width="9.42578125" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+    <col min="11" max="12" width="12.7109375" customWidth="1"/>
     <col min="13" max="26" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17890,8 +18104,8 @@
       <c r="L3" s="11"/>
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B4" s="139" t="s">
-        <v>203</v>
+      <c r="B4" s="137" t="s">
+        <v>196</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="14"/>
@@ -17908,808 +18122,1379 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="88" t="s">
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G5" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I5" s="70">
+        <v>24</v>
+      </c>
+      <c r="J5" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K5" s="150" t="s">
+        <v>245</v>
+      </c>
+      <c r="L5" s="152" t="s">
+        <v>246</v>
+      </c>
+      <c r="N5" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="18"/>
-      <c r="N5" s="27" t="s">
-        <v>94</v>
-      </c>
     </row>
     <row r="6" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B6" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="C6" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="88" t="s">
-        <v>96</v>
-      </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="18"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G6" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I6" s="70">
+        <v>24</v>
+      </c>
+      <c r="J6" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K6" s="89">
+        <v>1.2731481481481483E-3</v>
+      </c>
+      <c r="L6" s="154" t="s">
+        <v>247</v>
+      </c>
       <c r="N6" s="27"/>
     </row>
     <row r="7" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B7" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="15" t="s">
+      <c r="B7" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="C7" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="89" t="s">
-        <v>98</v>
-      </c>
-      <c r="L7" s="18"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G7" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I7" s="70">
+        <v>24</v>
+      </c>
+      <c r="J7" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7" s="150" t="s">
+        <v>248</v>
+      </c>
+      <c r="L7" s="154" t="s">
+        <v>249</v>
+      </c>
       <c r="N7" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B8" s="13" t="s">
-        <v>99</v>
+      <c r="B8" s="29" t="s">
+        <v>242</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="88" t="s">
-        <v>100</v>
-      </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="18"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G8" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H8" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I8" s="70">
+        <v>24</v>
+      </c>
+      <c r="J8" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8" s="150" t="s">
+        <v>250</v>
+      </c>
+      <c r="L8" s="154" t="s">
+        <v>251</v>
+      </c>
       <c r="N8" s="27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="13.5" customHeight="1">
+      <c r="B9" s="136" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B9" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="88" t="s">
-        <v>102</v>
-      </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="18"/>
+      <c r="D9" s="132"/>
+      <c r="E9" s="132"/>
+      <c r="F9" s="147" t="s">
+        <v>214</v>
+      </c>
+      <c r="G9" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I9" s="70">
+        <v>24</v>
+      </c>
+      <c r="J9" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K9" s="150" t="s">
+        <v>253</v>
+      </c>
+      <c r="L9" s="154" t="s">
+        <v>254</v>
+      </c>
       <c r="N9" s="27"/>
     </row>
     <row r="10" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B10" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" s="15" t="s">
+      <c r="B10" s="136" t="s">
+        <v>252</v>
+      </c>
+      <c r="C10" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="18"/>
+      <c r="D10" s="132"/>
+      <c r="E10" s="132"/>
+      <c r="F10" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G10" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H10" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I10" s="70">
+        <v>24</v>
+      </c>
+      <c r="J10" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K10" s="150" t="s">
+        <v>255</v>
+      </c>
+      <c r="L10" s="154" t="s">
+        <v>256</v>
+      </c>
       <c r="N10" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B11" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="C11" s="15" t="s">
+      <c r="B11" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="90"/>
+      <c r="D11" s="132"/>
+      <c r="E11" s="132"/>
+      <c r="F11" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G11" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H11" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I11" s="70">
+        <v>24</v>
+      </c>
+      <c r="J11" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11" s="150" t="s">
+        <v>261</v>
+      </c>
+      <c r="L11" s="154" t="s">
+        <v>262</v>
+      </c>
       <c r="N11" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B12" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" s="15" t="s">
+      <c r="B12" s="136" t="s">
+        <v>257</v>
+      </c>
+      <c r="C12" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="88" t="s">
-        <v>106</v>
-      </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="90"/>
+      <c r="D12" s="132"/>
+      <c r="E12" s="132"/>
+      <c r="F12" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G12" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H12" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I12" s="70">
+        <v>24</v>
+      </c>
+      <c r="J12" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K12" s="150" t="s">
+        <v>263</v>
+      </c>
+      <c r="L12" s="154" t="s">
+        <v>264</v>
+      </c>
       <c r="N12" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B13" s="138" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" s="59" t="s">
+      <c r="B13" s="136" t="s">
+        <v>258</v>
+      </c>
+      <c r="C13" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="68"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="88" t="s">
-        <v>108</v>
-      </c>
-      <c r="G13" s="68"/>
-      <c r="H13" s="68"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="68"/>
-      <c r="K13" s="91"/>
-      <c r="L13" s="92"/>
+      <c r="D13" s="132"/>
+      <c r="E13" s="132"/>
+      <c r="F13" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G13" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I13" s="70">
+        <v>24</v>
+      </c>
+      <c r="J13" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K13" s="150" t="s">
+        <v>265</v>
+      </c>
+      <c r="L13" s="154" t="s">
+        <v>266</v>
+      </c>
       <c r="M13" s="78"/>
       <c r="N13" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B14" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="C14" s="59" t="s">
+      <c r="B14" s="136" t="s">
+        <v>259</v>
+      </c>
+      <c r="C14" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="68"/>
-      <c r="H14" s="68"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="68"/>
-      <c r="K14" s="91"/>
-      <c r="L14" s="92"/>
+      <c r="D14" s="132"/>
+      <c r="E14" s="132"/>
+      <c r="F14" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G14" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H14" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I14" s="70">
+        <v>24</v>
+      </c>
+      <c r="J14" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K14" s="17">
+        <v>7.4884259259259262E-3</v>
+      </c>
+      <c r="L14" s="154" t="s">
+        <v>267</v>
+      </c>
       <c r="M14" s="78"/>
       <c r="N14" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B15" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="C15" s="25" t="s">
+      <c r="B15" s="136" t="s">
+        <v>260</v>
+      </c>
+      <c r="C15" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="92"/>
+      <c r="D15" s="132"/>
+      <c r="E15" s="132"/>
+      <c r="F15" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G15" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H15" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I15" s="70">
+        <v>24</v>
+      </c>
+      <c r="J15" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K15" s="157" t="s">
+        <v>268</v>
+      </c>
+      <c r="L15" s="154" t="s">
+        <v>269</v>
+      </c>
       <c r="N15" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B16" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="C16" s="25" t="s">
+      <c r="B16" s="136" t="s">
+        <v>270</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="88" t="s">
-        <v>112</v>
-      </c>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="92"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G16" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I16" s="70">
+        <v>24</v>
+      </c>
+      <c r="J16" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K16" s="157" t="s">
+        <v>272</v>
+      </c>
+      <c r="L16" s="154" t="s">
+        <v>273</v>
+      </c>
       <c r="N16" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B17" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C17" s="25" t="s">
+      <c r="B17" s="136" t="s">
+        <v>271</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="88" t="s">
-        <v>114</v>
-      </c>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="92"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G17" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H17" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I17" s="70">
+        <v>24</v>
+      </c>
+      <c r="J17" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K17" s="157" t="s">
+        <v>274</v>
+      </c>
+      <c r="L17" s="154" t="s">
+        <v>275</v>
+      </c>
       <c r="N17" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B18" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="C18" s="25" t="s">
+      <c r="B18" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="92"/>
+      <c r="D18" s="132"/>
+      <c r="E18" s="132"/>
+      <c r="F18" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G18" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H18" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I18" s="70">
+        <v>24</v>
+      </c>
+      <c r="J18" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K18" s="157" t="s">
+        <v>282</v>
+      </c>
+      <c r="L18" s="154" t="s">
+        <v>283</v>
+      </c>
       <c r="N18" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B19" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="C19" s="25" t="s">
+      <c r="B19" s="136" t="s">
+        <v>276</v>
+      </c>
+      <c r="C19" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="92"/>
+      <c r="D19" s="132"/>
+      <c r="E19" s="132"/>
+      <c r="F19" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G19" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I19" s="70">
+        <v>24</v>
+      </c>
+      <c r="J19" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K19" s="157" t="s">
+        <v>284</v>
+      </c>
+      <c r="L19" s="154" t="s">
+        <v>285</v>
+      </c>
       <c r="N19" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B20" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="C20" s="25" t="s">
+      <c r="B20" s="136" t="s">
+        <v>277</v>
+      </c>
+      <c r="C20" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="92"/>
+      <c r="D20" s="132"/>
+      <c r="E20" s="132"/>
+      <c r="F20" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G20" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H20" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I20" s="70">
+        <v>24</v>
+      </c>
+      <c r="J20" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K20" s="157" t="s">
+        <v>286</v>
+      </c>
+      <c r="L20" s="154" t="s">
+        <v>287</v>
+      </c>
       <c r="N20" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B21" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="C21" s="25" t="s">
+      <c r="B21" s="136" t="s">
+        <v>278</v>
+      </c>
+      <c r="C21" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="88" t="s">
-        <v>119</v>
-      </c>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="92"/>
+      <c r="D21" s="132"/>
+      <c r="E21" s="132"/>
+      <c r="F21" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G21" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H21" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I21" s="70">
+        <v>24</v>
+      </c>
+      <c r="J21" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K21" s="157" t="s">
+        <v>288</v>
+      </c>
+      <c r="L21" s="154" t="s">
+        <v>289</v>
+      </c>
       <c r="N21" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B22" s="140" t="s">
-        <v>204</v>
-      </c>
-      <c r="C22" s="25" t="s">
+      <c r="B22" s="136" t="s">
+        <v>279</v>
+      </c>
+      <c r="C22" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="118" t="s">
-        <v>221</v>
-      </c>
-      <c r="G22" s="25" t="s">
+      <c r="D22" s="132"/>
+      <c r="E22" s="132"/>
+      <c r="F22" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G22" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H22" s="93">
-        <v>43607</v>
-      </c>
-      <c r="I22" s="25">
+      <c r="H22" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I22" s="70">
         <v>24</v>
       </c>
-      <c r="J22" s="25">
-        <v>1</v>
-      </c>
-      <c r="K22" s="26">
-        <v>4.5138888888888887E-4</v>
-      </c>
-      <c r="L22" s="94" t="s">
-        <v>120</v>
+      <c r="J22" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K22" s="157" t="s">
+        <v>290</v>
+      </c>
+      <c r="L22" s="154" t="s">
+        <v>291</v>
       </c>
       <c r="N22" s="27"/>
     </row>
     <row r="23" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B23" s="140" t="s">
-        <v>205</v>
-      </c>
-      <c r="C23" s="25" t="s">
+      <c r="B23" s="136" t="s">
+        <v>280</v>
+      </c>
+      <c r="C23" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="149" t="s">
-        <v>222</v>
-      </c>
-      <c r="G23" s="25" t="s">
+      <c r="D23" s="132"/>
+      <c r="E23" s="132"/>
+      <c r="F23" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G23" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H23" s="93">
-        <v>43607</v>
-      </c>
-      <c r="I23" s="25">
+      <c r="H23" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I23" s="70">
         <v>24</v>
       </c>
-      <c r="J23" s="25">
-        <v>1</v>
-      </c>
-      <c r="K23" s="26">
-        <v>2.4305555555555555E-4</v>
-      </c>
-      <c r="L23" s="94" t="s">
-        <v>121</v>
+      <c r="J23" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K23" s="157" t="s">
+        <v>292</v>
+      </c>
+      <c r="L23" s="154" t="s">
+        <v>293</v>
       </c>
       <c r="N23" s="27"/>
     </row>
     <row r="24" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B24" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="C24" s="25" t="s">
+      <c r="B24" s="136" t="s">
+        <v>281</v>
+      </c>
+      <c r="C24" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="88" t="s">
-        <v>123</v>
-      </c>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="92"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G24" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H24" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I24" s="70">
+        <v>24</v>
+      </c>
+      <c r="J24" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K24" s="157" t="s">
+        <v>294</v>
+      </c>
+      <c r="L24" s="154" t="s">
+        <v>295</v>
+      </c>
       <c r="N24" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="2:14" ht="13.5" customHeight="1">
       <c r="B25" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="C25" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="88" t="s">
-        <v>125</v>
-      </c>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="92"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="156"/>
+      <c r="L25" s="153"/>
       <c r="N25" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="2:14" ht="13.5" customHeight="1">
       <c r="B26" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="C26" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="64"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="24"/>
-      <c r="L26" s="92"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="156"/>
+      <c r="L26" s="153"/>
       <c r="N26" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B27" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="C27" s="25" t="s">
+      <c r="B27" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="25"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="91"/>
-      <c r="L27" s="92"/>
+      <c r="D27" s="132"/>
+      <c r="E27" s="132"/>
+      <c r="F27" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G27" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H27" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I27" s="70">
+        <v>24</v>
+      </c>
+      <c r="J27" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K27" s="157" t="s">
+        <v>300</v>
+      </c>
+      <c r="L27" s="154" t="s">
+        <v>301</v>
+      </c>
       <c r="M27" s="78"/>
       <c r="N27" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B28" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="C28" s="25" t="s">
+      <c r="B28" s="136" t="s">
+        <v>296</v>
+      </c>
+      <c r="C28" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="15"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="68"/>
-      <c r="H28" s="68"/>
-      <c r="I28" s="68"/>
-      <c r="J28" s="68"/>
-      <c r="K28" s="91"/>
-      <c r="L28" s="92"/>
+      <c r="D28" s="132"/>
+      <c r="E28" s="132"/>
+      <c r="F28" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G28" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H28" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I28" s="70">
+        <v>24</v>
+      </c>
+      <c r="J28" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K28" s="157" t="s">
+        <v>302</v>
+      </c>
+      <c r="L28" s="154" t="s">
+        <v>303</v>
+      </c>
       <c r="M28" s="78"/>
       <c r="N28" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B29" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="C29" s="25" t="s">
+      <c r="B29" s="136" t="s">
+        <v>297</v>
+      </c>
+      <c r="C29" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="15"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="64"/>
-      <c r="G29" s="68"/>
-      <c r="H29" s="68"/>
-      <c r="I29" s="68"/>
-      <c r="J29" s="68"/>
-      <c r="K29" s="91"/>
-      <c r="L29" s="92"/>
+      <c r="D29" s="132"/>
+      <c r="E29" s="132"/>
+      <c r="F29" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G29" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H29" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I29" s="70">
+        <v>24</v>
+      </c>
+      <c r="J29" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K29" s="157" t="s">
+        <v>284</v>
+      </c>
+      <c r="L29" s="154" t="s">
+        <v>304</v>
+      </c>
       <c r="M29" s="78"/>
       <c r="N29" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B30" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="C30" s="25" t="s">
+      <c r="B30" s="136" t="s">
+        <v>298</v>
+      </c>
+      <c r="C30" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="68"/>
-      <c r="E30" s="68"/>
-      <c r="F30" s="88" t="s">
-        <v>131</v>
-      </c>
-      <c r="G30" s="68"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="68"/>
-      <c r="J30" s="68"/>
-      <c r="K30" s="91"/>
-      <c r="L30" s="92"/>
+      <c r="D30" s="132"/>
+      <c r="E30" s="132"/>
+      <c r="F30" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G30" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H30" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I30" s="70">
+        <v>24</v>
+      </c>
+      <c r="J30" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K30" s="157" t="s">
+        <v>305</v>
+      </c>
+      <c r="L30" s="154" t="s">
+        <v>306</v>
+      </c>
       <c r="M30" s="78"/>
       <c r="N30" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B31" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C31" s="25" t="s">
+      <c r="B31" s="136" t="s">
+        <v>299</v>
+      </c>
+      <c r="C31" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D31" s="68"/>
-      <c r="E31" s="68"/>
-      <c r="F31" s="88" t="s">
-        <v>131</v>
-      </c>
-      <c r="G31" s="68"/>
-      <c r="H31" s="68"/>
-      <c r="I31" s="68"/>
-      <c r="J31" s="68"/>
-      <c r="K31" s="91"/>
-      <c r="L31" s="92"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G31" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H31" s="155">
+        <v>22.05</v>
+      </c>
+      <c r="I31" s="70">
+        <v>24</v>
+      </c>
+      <c r="J31" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K31" s="157" t="s">
+        <v>307</v>
+      </c>
+      <c r="L31" s="154" t="s">
+        <v>308</v>
+      </c>
       <c r="M31" s="78"/>
       <c r="N31" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B32" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="C32" s="25" t="s">
+      <c r="B32" s="136" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" s="59" t="s">
         <v>10</v>
       </c>
       <c r="D32" s="68"/>
       <c r="E32" s="68"/>
       <c r="F32" s="88" t="s">
-        <v>131</v>
+        <v>101</v>
       </c>
       <c r="G32" s="68"/>
       <c r="H32" s="68"/>
       <c r="I32" s="68"/>
       <c r="J32" s="68"/>
-      <c r="K32" s="91"/>
-      <c r="L32" s="92"/>
+      <c r="K32" s="149"/>
+      <c r="L32" s="159"/>
       <c r="M32" s="78"/>
       <c r="N32" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B33" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="C33" s="83" t="s">
+      <c r="B33" s="158" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="80"/>
-      <c r="E33" s="80"/>
-      <c r="F33" s="95" t="s">
-        <v>135</v>
-      </c>
-      <c r="G33" s="80"/>
-      <c r="H33" s="80"/>
-      <c r="I33" s="80"/>
-      <c r="J33" s="80"/>
-      <c r="K33" s="96"/>
-      <c r="L33" s="97"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="68"/>
+      <c r="F33" s="64"/>
+      <c r="G33" s="68"/>
+      <c r="H33" s="68"/>
+      <c r="I33" s="68"/>
+      <c r="J33" s="68"/>
+      <c r="K33" s="149"/>
+      <c r="L33" s="151"/>
       <c r="M33" s="78"/>
       <c r="N33" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B34" s="98"/>
-      <c r="C34" s="78">
-        <f t="shared" ref="C34:E34" si="0">COUNTA(C4:C33)</f>
-        <v>29</v>
-      </c>
-      <c r="D34" s="78">
-        <f t="shared" si="0"/>
+      <c r="B34" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="64"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="90"/>
+      <c r="M34" s="78"/>
+    </row>
+    <row r="35" spans="2:14" ht="13.5" customHeight="1">
+      <c r="B35" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="88" t="s">
+        <v>105</v>
+      </c>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
+      <c r="L35" s="90"/>
+    </row>
+    <row r="36" spans="2:14" ht="13.5" customHeight="1">
+      <c r="B36" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="88" t="s">
+        <v>107</v>
+      </c>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="24"/>
+      <c r="L36" s="90"/>
+    </row>
+    <row r="37" spans="2:14" ht="13.5" customHeight="1">
+      <c r="B37" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="64"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
+      <c r="L37" s="90"/>
+    </row>
+    <row r="38" spans="2:14" ht="13.5" customHeight="1">
+      <c r="B38" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="64"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="24"/>
+      <c r="K38" s="24"/>
+      <c r="L38" s="90"/>
+    </row>
+    <row r="39" spans="2:14" ht="13.5" customHeight="1">
+      <c r="B39" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="64"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24"/>
+      <c r="K39" s="24"/>
+      <c r="L39" s="90"/>
+    </row>
+    <row r="40" spans="2:14" ht="13.5" customHeight="1">
+      <c r="B40" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="88" t="s">
+        <v>112</v>
+      </c>
+      <c r="G40" s="24"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24"/>
+      <c r="K40" s="24"/>
+      <c r="L40" s="90"/>
+    </row>
+    <row r="41" spans="2:14" ht="13.5" customHeight="1">
+      <c r="B41" s="138" t="s">
+        <v>197</v>
+      </c>
+      <c r="C41" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="G41" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="H41" s="91">
+        <v>43607</v>
+      </c>
+      <c r="I41" s="25">
+        <v>24</v>
+      </c>
+      <c r="J41" s="25">
+        <v>1</v>
+      </c>
+      <c r="K41" s="26">
+        <v>4.5138888888888887E-4</v>
+      </c>
+      <c r="L41" s="92" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" ht="13.5" customHeight="1">
+      <c r="B42" s="138" t="s">
+        <v>198</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="147" t="s">
+        <v>215</v>
+      </c>
+      <c r="G42" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="H42" s="91">
+        <v>43607</v>
+      </c>
+      <c r="I42" s="25">
+        <v>24</v>
+      </c>
+      <c r="J42" s="25">
+        <v>1</v>
+      </c>
+      <c r="K42" s="26">
+        <v>2.4305555555555555E-4</v>
+      </c>
+      <c r="L42" s="92" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" ht="13.5" customHeight="1">
+      <c r="B43" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="88" t="s">
+        <v>116</v>
+      </c>
+      <c r="G43" s="24"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="24"/>
+      <c r="J43" s="24"/>
+      <c r="K43" s="24"/>
+      <c r="L43" s="90"/>
+    </row>
+    <row r="44" spans="2:14" ht="13.5" customHeight="1">
+      <c r="B44" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C44" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="88" t="s">
+        <v>118</v>
+      </c>
+      <c r="G44" s="24"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24"/>
+      <c r="K44" s="24"/>
+      <c r="L44" s="90"/>
+    </row>
+    <row r="45" spans="2:14" ht="13.5" customHeight="1">
+      <c r="B45" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C45" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="64"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="24"/>
+      <c r="J45" s="24"/>
+      <c r="K45" s="24"/>
+      <c r="L45" s="90"/>
+    </row>
+    <row r="46" spans="2:14" ht="13.5" customHeight="1">
+      <c r="B46" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C46" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="25"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="64"/>
+      <c r="G46" s="68"/>
+      <c r="H46" s="68"/>
+      <c r="I46" s="68"/>
+      <c r="J46" s="68"/>
+      <c r="K46" s="89"/>
+      <c r="L46" s="90"/>
+    </row>
+    <row r="47" spans="2:14" ht="13.5" customHeight="1">
+      <c r="B47" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C47" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" s="15"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="64"/>
+      <c r="G47" s="68"/>
+      <c r="H47" s="68"/>
+      <c r="I47" s="68"/>
+      <c r="J47" s="68"/>
+      <c r="K47" s="89"/>
+      <c r="L47" s="90"/>
+    </row>
+    <row r="48" spans="2:14" ht="13.5" customHeight="1">
+      <c r="B48" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="C48" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" s="15"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="64"/>
+      <c r="G48" s="68"/>
+      <c r="H48" s="68"/>
+      <c r="I48" s="68"/>
+      <c r="J48" s="68"/>
+      <c r="K48" s="89"/>
+      <c r="L48" s="90"/>
+    </row>
+    <row r="49" spans="2:12" ht="13.5" customHeight="1">
+      <c r="B49" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C49" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" s="68"/>
+      <c r="E49" s="68"/>
+      <c r="F49" s="88" t="s">
+        <v>124</v>
+      </c>
+      <c r="G49" s="68"/>
+      <c r="H49" s="68"/>
+      <c r="I49" s="68"/>
+      <c r="J49" s="68"/>
+      <c r="K49" s="89"/>
+      <c r="L49" s="90"/>
+    </row>
+    <row r="50" spans="2:12" ht="13.5" customHeight="1">
+      <c r="B50" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C50" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" s="68"/>
+      <c r="E50" s="68"/>
+      <c r="F50" s="88" t="s">
+        <v>124</v>
+      </c>
+      <c r="G50" s="68"/>
+      <c r="H50" s="68"/>
+      <c r="I50" s="68"/>
+      <c r="J50" s="68"/>
+      <c r="K50" s="89"/>
+      <c r="L50" s="90"/>
+    </row>
+    <row r="51" spans="2:12" ht="13.5" customHeight="1">
+      <c r="B51" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C51" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" s="68"/>
+      <c r="E51" s="68"/>
+      <c r="F51" s="88" t="s">
+        <v>124</v>
+      </c>
+      <c r="G51" s="68"/>
+      <c r="H51" s="68"/>
+      <c r="I51" s="68"/>
+      <c r="J51" s="68"/>
+      <c r="K51" s="89"/>
+      <c r="L51" s="90"/>
+    </row>
+    <row r="52" spans="2:12" ht="13.5" customHeight="1" thickBot="1">
+      <c r="B52" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="C52" s="83" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" s="80"/>
+      <c r="E52" s="80"/>
+      <c r="F52" s="93" t="s">
+        <v>128</v>
+      </c>
+      <c r="G52" s="80"/>
+      <c r="H52" s="80"/>
+      <c r="I52" s="80"/>
+      <c r="J52" s="80"/>
+      <c r="K52" s="94"/>
+      <c r="L52" s="95"/>
+    </row>
+    <row r="53" spans="2:12" ht="13.5" customHeight="1">
+      <c r="B53" s="96"/>
+      <c r="C53" s="78">
+        <f>COUNTA(C4:C52)</f>
+        <v>48</v>
+      </c>
+      <c r="D53" s="78">
+        <f>COUNTA(D4:D52)</f>
         <v>0</v>
       </c>
-      <c r="E34" s="78">
-        <f t="shared" si="0"/>
+      <c r="E53" s="78">
+        <f>COUNTA(E4:E52)</f>
         <v>0</v>
       </c>
-      <c r="F34" s="78"/>
-      <c r="G34" s="78"/>
-      <c r="H34" s="78"/>
-      <c r="I34" s="78"/>
-      <c r="J34" s="78"/>
-      <c r="K34" s="78"/>
-      <c r="L34" s="78"/>
-      <c r="M34" s="78"/>
-    </row>
-    <row r="35" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B35" s="98"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
-    </row>
-    <row r="36" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B36" s="98"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
-    </row>
-    <row r="37" spans="2:14" ht="13.5" customHeight="1"/>
-    <row r="38" spans="2:14" ht="13.5" customHeight="1">
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="38"/>
-    </row>
-    <row r="39" spans="2:14" ht="13.5" customHeight="1">
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
-    </row>
-    <row r="40" spans="2:14" ht="13.5" customHeight="1">
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38"/>
-    </row>
-    <row r="41" spans="2:14" ht="13.5" customHeight="1">
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
-    </row>
-    <row r="42" spans="2:14" ht="13.5" customHeight="1">
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38"/>
-    </row>
-    <row r="43" spans="2:14" ht="13.5" customHeight="1">
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="38"/>
-    </row>
-    <row r="44" spans="2:14" ht="13.5" customHeight="1">
-      <c r="C44" s="38"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="38"/>
-    </row>
-    <row r="45" spans="2:14" ht="13.5" customHeight="1">
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-    </row>
-    <row r="46" spans="2:14" ht="13.5" customHeight="1">
-      <c r="C46" s="38"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
-    </row>
-    <row r="47" spans="2:14" ht="13.5" customHeight="1">
-      <c r="C47" s="38"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="38"/>
-    </row>
-    <row r="48" spans="2:14" ht="13.5" customHeight="1">
-      <c r="C48" s="38"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="38"/>
-    </row>
-    <row r="49" spans="3:5" ht="13.5" customHeight="1">
-      <c r="C49" s="38"/>
-      <c r="D49" s="38"/>
-      <c r="E49" s="38"/>
-    </row>
-    <row r="50" spans="3:5" ht="13.5" customHeight="1">
-      <c r="C50" s="38"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="38"/>
-    </row>
-    <row r="51" spans="3:5" ht="13.5" customHeight="1">
-      <c r="C51" s="38"/>
-      <c r="D51" s="38"/>
-      <c r="E51" s="38"/>
-    </row>
-    <row r="52" spans="3:5" ht="13.5" customHeight="1">
-      <c r="C52" s="38"/>
-      <c r="D52" s="38"/>
-      <c r="E52" s="38"/>
-    </row>
-    <row r="53" spans="3:5" ht="13.5" customHeight="1">
-      <c r="C53" s="38"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="38"/>
-    </row>
-    <row r="54" spans="3:5" ht="13.5" customHeight="1">
+      <c r="F53" s="78"/>
+      <c r="G53" s="78"/>
+      <c r="H53" s="78"/>
+      <c r="I53" s="78"/>
+      <c r="J53" s="78"/>
+      <c r="K53" s="78"/>
+      <c r="L53" s="78"/>
+    </row>
+    <row r="54" spans="2:12" ht="13.5" customHeight="1">
+      <c r="B54" s="96"/>
       <c r="C54" s="38"/>
       <c r="D54" s="38"/>
       <c r="E54" s="38"/>
     </row>
-    <row r="55" spans="3:5" ht="13.5" customHeight="1">
+    <row r="55" spans="2:12" ht="13.5" customHeight="1">
+      <c r="B55" s="96"/>
       <c r="C55" s="38"/>
       <c r="D55" s="38"/>
       <c r="E55" s="38"/>
     </row>
-    <row r="56" spans="3:5" ht="13.5" customHeight="1">
-      <c r="C56" s="38"/>
-      <c r="D56" s="38"/>
-      <c r="E56" s="38"/>
-    </row>
-    <row r="57" spans="3:5" ht="13.5" customHeight="1">
+    <row r="56" spans="2:12" ht="13.5" customHeight="1"/>
+    <row r="57" spans="2:12" ht="13.5" customHeight="1">
       <c r="C57" s="38"/>
       <c r="D57" s="38"/>
       <c r="E57" s="38"/>
     </row>
-    <row r="58" spans="3:5" ht="13.5" customHeight="1">
+    <row r="58" spans="2:12" ht="13.5" customHeight="1">
       <c r="C58" s="38"/>
       <c r="D58" s="38"/>
       <c r="E58" s="38"/>
     </row>
-    <row r="59" spans="3:5" ht="13.5" customHeight="1">
+    <row r="59" spans="2:12" ht="13.5" customHeight="1">
       <c r="C59" s="38"/>
       <c r="D59" s="38"/>
       <c r="E59" s="38"/>
     </row>
-    <row r="60" spans="3:5" ht="13.5" customHeight="1">
+    <row r="60" spans="2:12" ht="13.5" customHeight="1">
       <c r="C60" s="38"/>
       <c r="D60" s="38"/>
       <c r="E60" s="38"/>
     </row>
-    <row r="61" spans="3:5" ht="13.5" customHeight="1">
+    <row r="61" spans="2:12" ht="13.5" customHeight="1">
       <c r="C61" s="38"/>
       <c r="D61" s="38"/>
       <c r="E61" s="38"/>
     </row>
-    <row r="62" spans="3:5" ht="13.5" customHeight="1">
+    <row r="62" spans="2:12" ht="13.5" customHeight="1">
       <c r="C62" s="38"/>
       <c r="D62" s="38"/>
       <c r="E62" s="38"/>
     </row>
-    <row r="63" spans="3:5" ht="13.5" customHeight="1">
+    <row r="63" spans="2:12" ht="13.5" customHeight="1">
       <c r="C63" s="38"/>
       <c r="D63" s="38"/>
       <c r="E63" s="38"/>
     </row>
-    <row r="64" spans="3:5" ht="13.5" customHeight="1">
+    <row r="64" spans="2:12" ht="13.5" customHeight="1">
       <c r="C64" s="38"/>
       <c r="D64" s="38"/>
       <c r="E64" s="38"/>
@@ -23449,28 +24234,118 @@
       <c r="D1011" s="38"/>
       <c r="E1011" s="38"/>
     </row>
+    <row r="1012" spans="3:5" ht="15" customHeight="1">
+      <c r="C1012" s="38"/>
+      <c r="D1012" s="38"/>
+      <c r="E1012" s="38"/>
+    </row>
+    <row r="1013" spans="3:5" ht="15" customHeight="1">
+      <c r="C1013" s="38"/>
+      <c r="D1013" s="38"/>
+      <c r="E1013" s="38"/>
+    </row>
+    <row r="1014" spans="3:5" ht="15" customHeight="1">
+      <c r="C1014" s="38"/>
+      <c r="D1014" s="38"/>
+      <c r="E1014" s="38"/>
+    </row>
+    <row r="1015" spans="3:5" ht="15" customHeight="1">
+      <c r="C1015" s="38"/>
+      <c r="D1015" s="38"/>
+      <c r="E1015" s="38"/>
+    </row>
+    <row r="1016" spans="3:5" ht="15" customHeight="1">
+      <c r="C1016" s="38"/>
+      <c r="D1016" s="38"/>
+      <c r="E1016" s="38"/>
+    </row>
+    <row r="1017" spans="3:5" ht="15" customHeight="1">
+      <c r="C1017" s="38"/>
+      <c r="D1017" s="38"/>
+      <c r="E1017" s="38"/>
+    </row>
+    <row r="1018" spans="3:5" ht="15" customHeight="1">
+      <c r="C1018" s="38"/>
+      <c r="D1018" s="38"/>
+      <c r="E1018" s="38"/>
+    </row>
+    <row r="1019" spans="3:5" ht="15" customHeight="1">
+      <c r="C1019" s="38"/>
+      <c r="D1019" s="38"/>
+      <c r="E1019" s="38"/>
+    </row>
+    <row r="1020" spans="3:5" ht="15" customHeight="1">
+      <c r="C1020" s="38"/>
+      <c r="D1020" s="38"/>
+      <c r="E1020" s="38"/>
+    </row>
+    <row r="1021" spans="3:5" ht="15" customHeight="1">
+      <c r="C1021" s="38"/>
+      <c r="D1021" s="38"/>
+      <c r="E1021" s="38"/>
+    </row>
+    <row r="1022" spans="3:5" ht="15" customHeight="1">
+      <c r="C1022" s="38"/>
+      <c r="D1022" s="38"/>
+      <c r="E1022" s="38"/>
+    </row>
+    <row r="1023" spans="3:5" ht="15" customHeight="1">
+      <c r="C1023" s="38"/>
+      <c r="D1023" s="38"/>
+      <c r="E1023" s="38"/>
+    </row>
+    <row r="1024" spans="3:5" ht="15" customHeight="1">
+      <c r="C1024" s="38"/>
+      <c r="D1024" s="38"/>
+      <c r="E1024" s="38"/>
+    </row>
+    <row r="1025" spans="3:5" ht="15" customHeight="1">
+      <c r="C1025" s="38"/>
+      <c r="D1025" s="38"/>
+      <c r="E1025" s="38"/>
+    </row>
+    <row r="1026" spans="3:5" ht="15" customHeight="1">
+      <c r="C1026" s="38"/>
+      <c r="D1026" s="38"/>
+      <c r="E1026" s="38"/>
+    </row>
+    <row r="1027" spans="3:5" ht="15" customHeight="1">
+      <c r="C1027" s="38"/>
+      <c r="D1027" s="38"/>
+      <c r="E1027" s="38"/>
+    </row>
+    <row r="1028" spans="3:5" ht="15" customHeight="1">
+      <c r="C1028" s="38"/>
+      <c r="D1028" s="38"/>
+      <c r="E1028" s="38"/>
+    </row>
+    <row r="1029" spans="3:5" ht="15" customHeight="1">
+      <c r="C1029" s="38"/>
+      <c r="D1029" s="38"/>
+      <c r="E1029" s="38"/>
+    </row>
+    <row r="1030" spans="3:5" ht="15" customHeight="1">
+      <c r="C1030" s="38"/>
+      <c r="D1030" s="38"/>
+      <c r="E1030" s="38"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1"/>
-    <hyperlink ref="F6" r:id="rId2"/>
-    <hyperlink ref="F8" r:id="rId3"/>
-    <hyperlink ref="F9" r:id="rId4"/>
-    <hyperlink ref="F12" r:id="rId5"/>
-    <hyperlink ref="F13" r:id="rId6"/>
-    <hyperlink ref="F16" r:id="rId7"/>
-    <hyperlink ref="F17" r:id="rId8"/>
-    <hyperlink ref="F21" r:id="rId9"/>
-    <hyperlink ref="F24" r:id="rId10"/>
-    <hyperlink ref="F25" r:id="rId11"/>
-    <hyperlink ref="F30" r:id="rId12"/>
-    <hyperlink ref="F31" r:id="rId13"/>
-    <hyperlink ref="F32" r:id="rId14"/>
-    <hyperlink ref="F33" r:id="rId15"/>
-    <hyperlink ref="B22" r:id="rId16"/>
-    <hyperlink ref="B23" r:id="rId17"/>
+    <hyperlink ref="F32" r:id="rId1"/>
+    <hyperlink ref="F35" r:id="rId2"/>
+    <hyperlink ref="F36" r:id="rId3"/>
+    <hyperlink ref="F40" r:id="rId4"/>
+    <hyperlink ref="F43" r:id="rId5"/>
+    <hyperlink ref="F44" r:id="rId6"/>
+    <hyperlink ref="F49" r:id="rId7"/>
+    <hyperlink ref="F50" r:id="rId8"/>
+    <hyperlink ref="F51" r:id="rId9"/>
+    <hyperlink ref="F52" r:id="rId10"/>
+    <hyperlink ref="B41" r:id="rId11"/>
+    <hyperlink ref="B42" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -23499,7 +24374,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="13.5" customHeight="1">
       <c r="B1" s="37" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C1" s="38"/>
       <c r="D1" s="38"/>
@@ -23577,8 +24452,8 @@
       <c r="L3" s="11"/>
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B4" s="139" t="s">
-        <v>203</v>
+      <c r="B4" s="137" t="s">
+        <v>196</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="15"/>
@@ -23588,15 +24463,15 @@
       <c r="H4" s="38"/>
       <c r="I4" s="38"/>
       <c r="J4" s="38"/>
-      <c r="K4" s="110"/>
-      <c r="L4" s="111"/>
+      <c r="K4" s="108"/>
+      <c r="L4" s="109"/>
       <c r="N4" s="19" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="13.5" customHeight="1">
       <c r="B5" s="29" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="25" t="s">
@@ -23604,14 +24479,14 @@
       </c>
       <c r="E5" s="24"/>
       <c r="F5" s="24"/>
-      <c r="L5" s="111"/>
+      <c r="L5" s="109"/>
       <c r="N5" s="27" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="13.5" customHeight="1">
       <c r="B6" s="29" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="15" t="s">
@@ -23623,68 +24498,68 @@
       <c r="H6" s="36"/>
       <c r="I6" s="36"/>
       <c r="J6" s="36"/>
-      <c r="K6" s="112"/>
-      <c r="L6" s="111"/>
+      <c r="K6" s="110"/>
+      <c r="L6" s="109"/>
       <c r="N6" s="27" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="13.5" customHeight="1">
       <c r="B7" s="29" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="14"/>
-      <c r="F7" s="113"/>
-      <c r="G7" s="114"/>
-      <c r="H7" s="115"/>
-      <c r="I7" s="116"/>
-      <c r="J7" s="116"/>
-      <c r="K7" s="117"/>
-      <c r="L7" s="111"/>
+      <c r="F7" s="111"/>
+      <c r="G7" s="112"/>
+      <c r="H7" s="113"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="114"/>
+      <c r="K7" s="115"/>
+      <c r="L7" s="109"/>
       <c r="N7" s="27" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="13.5" customHeight="1">
       <c r="B8" s="29" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="14"/>
-      <c r="F8" s="118"/>
-      <c r="G8" s="119"/>
-      <c r="H8" s="119"/>
-      <c r="I8" s="119"/>
-      <c r="J8" s="119"/>
-      <c r="K8" s="120"/>
-      <c r="L8" s="121"/>
+      <c r="F8" s="116"/>
+      <c r="G8" s="117"/>
+      <c r="H8" s="117"/>
+      <c r="I8" s="117"/>
+      <c r="J8" s="117"/>
+      <c r="K8" s="118"/>
+      <c r="L8" s="119"/>
       <c r="N8" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="13.5" customHeight="1">
       <c r="B9" s="29" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C9" s="68"/>
       <c r="D9" s="59" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="68"/>
-      <c r="F9" s="122"/>
-      <c r="G9" s="123"/>
-      <c r="H9" s="123"/>
-      <c r="I9" s="123"/>
-      <c r="J9" s="123"/>
-      <c r="K9" s="124"/>
-      <c r="L9" s="125"/>
+      <c r="F9" s="120"/>
+      <c r="G9" s="121"/>
+      <c r="H9" s="121"/>
+      <c r="I9" s="121"/>
+      <c r="J9" s="121"/>
+      <c r="K9" s="122"/>
+      <c r="L9" s="123"/>
       <c r="M9" s="78"/>
       <c r="N9" s="27" t="s">
         <v>24</v>
@@ -23692,20 +24567,20 @@
     </row>
     <row r="10" spans="1:26" ht="13.5" customHeight="1">
       <c r="B10" s="29" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C10" s="68"/>
       <c r="D10" s="59" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="68"/>
-      <c r="F10" s="122"/>
-      <c r="G10" s="123"/>
-      <c r="H10" s="123"/>
-      <c r="I10" s="123"/>
-      <c r="J10" s="123"/>
-      <c r="K10" s="124"/>
-      <c r="L10" s="125"/>
+      <c r="F10" s="120"/>
+      <c r="G10" s="121"/>
+      <c r="H10" s="121"/>
+      <c r="I10" s="121"/>
+      <c r="J10" s="121"/>
+      <c r="K10" s="122"/>
+      <c r="L10" s="123"/>
       <c r="M10" s="78"/>
       <c r="N10" s="27" t="s">
         <v>24</v>
@@ -23713,20 +24588,20 @@
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1">
       <c r="B11" s="29" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C11" s="68"/>
       <c r="D11" s="59" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="68"/>
-      <c r="F11" s="126"/>
-      <c r="G11" s="114"/>
-      <c r="H11" s="114"/>
-      <c r="I11" s="114"/>
-      <c r="J11" s="114"/>
-      <c r="K11" s="127"/>
-      <c r="L11" s="128"/>
+      <c r="F11" s="124"/>
+      <c r="G11" s="112"/>
+      <c r="H11" s="112"/>
+      <c r="I11" s="112"/>
+      <c r="J11" s="112"/>
+      <c r="K11" s="125"/>
+      <c r="L11" s="126"/>
       <c r="M11" s="78"/>
       <c r="N11" s="27" t="s">
         <v>24</v>
@@ -23734,27 +24609,27 @@
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1">
       <c r="B12" s="29" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C12" s="24"/>
       <c r="D12" s="59" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="24"/>
-      <c r="F12" s="129"/>
-      <c r="G12" s="130"/>
-      <c r="H12" s="130"/>
-      <c r="I12" s="130"/>
-      <c r="J12" s="130"/>
-      <c r="K12" s="127"/>
-      <c r="L12" s="128"/>
+      <c r="F12" s="127"/>
+      <c r="G12" s="128"/>
+      <c r="H12" s="128"/>
+      <c r="I12" s="128"/>
+      <c r="J12" s="128"/>
+      <c r="K12" s="125"/>
+      <c r="L12" s="126"/>
       <c r="N12" s="27" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1">
       <c r="B13" s="13" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C13" s="24"/>
       <c r="D13" s="59"/>
@@ -23762,21 +24637,21 @@
         <v>12</v>
       </c>
       <c r="F13" s="60" t="s">
-        <v>185</v>
-      </c>
-      <c r="G13" s="130"/>
-      <c r="H13" s="130"/>
-      <c r="I13" s="130"/>
-      <c r="J13" s="130"/>
-      <c r="K13" s="130"/>
-      <c r="L13" s="128"/>
+        <v>178</v>
+      </c>
+      <c r="G13" s="128"/>
+      <c r="H13" s="128"/>
+      <c r="I13" s="128"/>
+      <c r="J13" s="128"/>
+      <c r="K13" s="128"/>
+      <c r="L13" s="126"/>
       <c r="N13" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="13.5" customHeight="1">
       <c r="B14" s="13" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="59"/>
@@ -23784,21 +24659,21 @@
         <v>12</v>
       </c>
       <c r="F14" s="60" t="s">
-        <v>187</v>
-      </c>
-      <c r="G14" s="114"/>
-      <c r="H14" s="115"/>
-      <c r="I14" s="116"/>
-      <c r="J14" s="116"/>
-      <c r="K14" s="117"/>
-      <c r="L14" s="128"/>
+        <v>180</v>
+      </c>
+      <c r="G14" s="112"/>
+      <c r="H14" s="113"/>
+      <c r="I14" s="114"/>
+      <c r="J14" s="114"/>
+      <c r="K14" s="115"/>
+      <c r="L14" s="126"/>
       <c r="N14" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1">
       <c r="B15" s="13" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="59"/>
@@ -23806,81 +24681,81 @@
         <v>12</v>
       </c>
       <c r="F15" s="60" t="s">
-        <v>189</v>
-      </c>
-      <c r="G15" s="130"/>
-      <c r="H15" s="130"/>
-      <c r="I15" s="130"/>
-      <c r="J15" s="130"/>
-      <c r="K15" s="130"/>
-      <c r="L15" s="128"/>
+        <v>182</v>
+      </c>
+      <c r="G15" s="128"/>
+      <c r="H15" s="128"/>
+      <c r="I15" s="128"/>
+      <c r="J15" s="128"/>
+      <c r="K15" s="128"/>
+      <c r="L15" s="126"/>
       <c r="N15" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1">
       <c r="B16" s="29" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C16" s="24"/>
       <c r="D16" s="25" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="24"/>
-      <c r="F16" s="129"/>
-      <c r="G16" s="130"/>
-      <c r="H16" s="130"/>
-      <c r="I16" s="130"/>
-      <c r="J16" s="130"/>
-      <c r="K16" s="130"/>
-      <c r="L16" s="125"/>
+      <c r="F16" s="127"/>
+      <c r="G16" s="128"/>
+      <c r="H16" s="128"/>
+      <c r="I16" s="128"/>
+      <c r="J16" s="128"/>
+      <c r="K16" s="128"/>
+      <c r="L16" s="123"/>
       <c r="N16" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="2:14" ht="13.5" customHeight="1">
       <c r="B17" s="29" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C17" s="24"/>
       <c r="D17" s="25" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="24"/>
-      <c r="F17" s="129"/>
-      <c r="G17" s="130"/>
-      <c r="H17" s="130"/>
-      <c r="I17" s="130"/>
-      <c r="J17" s="130"/>
-      <c r="K17" s="130"/>
-      <c r="L17" s="128"/>
+      <c r="F17" s="127"/>
+      <c r="G17" s="128"/>
+      <c r="H17" s="128"/>
+      <c r="I17" s="128"/>
+      <c r="J17" s="128"/>
+      <c r="K17" s="128"/>
+      <c r="L17" s="126"/>
       <c r="N17" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="2:14" ht="13.5" customHeight="1">
       <c r="B18" s="29" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C18" s="24"/>
       <c r="D18" s="25" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="24"/>
-      <c r="F18" s="129"/>
-      <c r="G18" s="130"/>
-      <c r="H18" s="130"/>
-      <c r="I18" s="130"/>
-      <c r="J18" s="130"/>
-      <c r="K18" s="130"/>
-      <c r="L18" s="128"/>
+      <c r="F18" s="127"/>
+      <c r="G18" s="128"/>
+      <c r="H18" s="128"/>
+      <c r="I18" s="128"/>
+      <c r="J18" s="128"/>
+      <c r="K18" s="128"/>
+      <c r="L18" s="126"/>
       <c r="N18" s="27" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="2:14" ht="13.5" customHeight="1">
       <c r="B19" s="13" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C19" s="24"/>
       <c r="D19" s="15" t="s">
@@ -23893,14 +24768,14 @@
       <c r="I19" s="71"/>
       <c r="J19" s="71"/>
       <c r="K19" s="71"/>
-      <c r="L19" s="128"/>
+      <c r="L19" s="126"/>
       <c r="N19" s="27" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="20" spans="2:14" ht="13.5" customHeight="1">
       <c r="B20" s="13" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C20" s="25" t="s">
         <v>10</v>
@@ -23912,15 +24787,15 @@
       <c r="H20" s="78"/>
       <c r="I20" s="78"/>
       <c r="J20" s="78"/>
-      <c r="K20" s="131"/>
-      <c r="L20" s="128"/>
+      <c r="K20" s="129"/>
+      <c r="L20" s="126"/>
       <c r="N20" s="27" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="2:14" ht="13.5" customHeight="1">
       <c r="B21" s="13" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C21" s="14"/>
       <c r="D21" s="15" t="s">
@@ -23933,36 +24808,36 @@
       <c r="I21" s="71"/>
       <c r="J21" s="71"/>
       <c r="K21" s="71"/>
-      <c r="L21" s="128"/>
+      <c r="L21" s="126"/>
       <c r="N21" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="2:14" ht="13.5" customHeight="1">
       <c r="B22" s="13" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="14"/>
-      <c r="F22" s="132" t="s">
-        <v>197</v>
+      <c r="F22" s="130" t="s">
+        <v>190</v>
       </c>
       <c r="G22" s="71"/>
       <c r="H22" s="71"/>
       <c r="I22" s="71"/>
       <c r="J22" s="71"/>
       <c r="K22" s="71"/>
-      <c r="L22" s="128"/>
+      <c r="L22" s="126"/>
       <c r="N22" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="2:14" ht="13.5" customHeight="1">
       <c r="B23" s="13" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="15" t="s">
@@ -23975,14 +24850,14 @@
       <c r="I23" s="71"/>
       <c r="J23" s="71"/>
       <c r="K23" s="71"/>
-      <c r="L23" s="128"/>
+      <c r="L23" s="126"/>
       <c r="N23" s="27" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="24" spans="2:14" ht="13.5" customHeight="1">
       <c r="B24" s="13" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="15" t="s">
@@ -23995,14 +24870,14 @@
       <c r="I24" s="71"/>
       <c r="J24" s="71"/>
       <c r="K24" s="71"/>
-      <c r="L24" s="125"/>
+      <c r="L24" s="123"/>
       <c r="N24" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="2:14" ht="13.5" customHeight="1">
       <c r="B25" s="13" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="15" t="s">
@@ -24010,14 +24885,14 @@
       </c>
       <c r="E25" s="14"/>
       <c r="F25" s="24"/>
-      <c r="L25" s="128"/>
+      <c r="L25" s="126"/>
       <c r="N25" s="27" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="2:14" ht="13.5" customHeight="1">
       <c r="B26" s="30" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C26" s="80"/>
       <c r="D26" s="83" t="s">
@@ -24025,19 +24900,19 @@
       </c>
       <c r="E26" s="80"/>
       <c r="F26" s="80"/>
-      <c r="G26" s="133"/>
-      <c r="H26" s="133"/>
-      <c r="I26" s="133"/>
-      <c r="J26" s="133"/>
-      <c r="K26" s="135"/>
-      <c r="L26" s="136"/>
+      <c r="G26" s="131"/>
+      <c r="H26" s="131"/>
+      <c r="I26" s="131"/>
+      <c r="J26" s="131"/>
+      <c r="K26" s="133"/>
+      <c r="L26" s="134"/>
       <c r="M26" s="78"/>
       <c r="N26" s="27" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B27" s="109"/>
+      <c r="B27" s="107"/>
       <c r="C27" s="78">
         <f t="shared" ref="C27:E27" si="0">COUNTA(C4:C26)</f>
         <v>1</v>
@@ -24060,7 +24935,7 @@
       <c r="M27" s="78"/>
     </row>
     <row r="28" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B28" s="109"/>
+      <c r="B28" s="107"/>
       <c r="C28" s="38"/>
       <c r="D28" s="38"/>
       <c r="E28" s="38"/>
@@ -28936,7 +29811,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="28.5" customHeight="1">
       <c r="B1" s="37" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C1" s="38"/>
       <c r="D1" s="38"/>
@@ -29013,50 +29888,50 @@
       <c r="L3" s="11"/>
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B4" s="139" t="s">
-        <v>203</v>
+      <c r="B4" s="137" t="s">
+        <v>196</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="14"/>
-      <c r="E4" s="134"/>
-      <c r="F4" s="134"/>
-      <c r="G4" s="134"/>
+      <c r="E4" s="132"/>
+      <c r="F4" s="132"/>
+      <c r="G4" s="132"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
-      <c r="K4" s="142"/>
-      <c r="L4" s="145"/>
+      <c r="K4" s="140"/>
+      <c r="L4" s="143"/>
     </row>
     <row r="5" spans="1:26" ht="13.5" customHeight="1">
       <c r="B5" s="13" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
-      <c r="F5" s="148"/>
+      <c r="F5" s="146"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
-      <c r="K5" s="142"/>
-      <c r="L5" s="145"/>
+      <c r="K5" s="140"/>
+      <c r="L5" s="143"/>
     </row>
     <row r="6" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B6" s="140" t="s">
-        <v>207</v>
+      <c r="B6" s="138" t="s">
+        <v>200</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="148" t="s">
-        <v>241</v>
-      </c>
-      <c r="G6" s="141" t="s">
+      <c r="F6" s="146" t="s">
+        <v>234</v>
+      </c>
+      <c r="G6" s="139" t="s">
         <v>18</v>
       </c>
       <c r="H6" s="14">
@@ -29068,492 +29943,492 @@
       <c r="J6" s="14">
         <v>1</v>
       </c>
-      <c r="K6" s="144" t="s">
-        <v>206</v>
-      </c>
-      <c r="L6" s="146" t="s">
-        <v>240</v>
+      <c r="K6" s="142" t="s">
+        <v>199</v>
+      </c>
+      <c r="L6" s="144" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B7" s="140" t="s">
-        <v>210</v>
+      <c r="B7" s="138" t="s">
+        <v>203</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
-      <c r="F7" s="148" t="s">
-        <v>241</v>
-      </c>
-      <c r="G7" s="141" t="s">
+      <c r="F7" s="146" t="s">
+        <v>234</v>
+      </c>
+      <c r="G7" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="134">
+      <c r="H7" s="132">
         <v>16</v>
       </c>
-      <c r="I7" s="134">
+      <c r="I7" s="132">
         <v>32</v>
       </c>
       <c r="J7" s="14">
         <v>1</v>
       </c>
-      <c r="K7" s="144" t="s">
-        <v>208</v>
-      </c>
-      <c r="L7" s="146" t="s">
-        <v>240</v>
+      <c r="K7" s="142" t="s">
+        <v>201</v>
+      </c>
+      <c r="L7" s="144" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B8" s="140" t="s">
-        <v>211</v>
+      <c r="B8" s="138" t="s">
+        <v>204</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
-      <c r="F8" s="148" t="s">
-        <v>241</v>
-      </c>
-      <c r="G8" s="141" t="s">
+      <c r="F8" s="146" t="s">
+        <v>234</v>
+      </c>
+      <c r="G8" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="134">
+      <c r="H8" s="132">
         <v>16</v>
       </c>
-      <c r="I8" s="134">
+      <c r="I8" s="132">
         <v>32</v>
       </c>
-      <c r="J8" s="134">
+      <c r="J8" s="132">
         <v>1</v>
       </c>
-      <c r="K8" s="144" t="s">
-        <v>209</v>
-      </c>
-      <c r="L8" s="146" t="s">
-        <v>240</v>
+      <c r="K8" s="142" t="s">
+        <v>202</v>
+      </c>
+      <c r="L8" s="144" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B9" s="140" t="s">
-        <v>212</v>
+      <c r="B9" s="138" t="s">
+        <v>205</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
-      <c r="F9" s="148" t="s">
-        <v>241</v>
-      </c>
-      <c r="G9" s="141" t="s">
+      <c r="F9" s="146" t="s">
+        <v>234</v>
+      </c>
+      <c r="G9" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="134">
+      <c r="H9" s="132">
         <v>16</v>
       </c>
-      <c r="I9" s="134">
+      <c r="I9" s="132">
         <v>32</v>
       </c>
-      <c r="J9" s="134">
+      <c r="J9" s="132">
         <v>1</v>
       </c>
-      <c r="K9" s="144" t="s">
-        <v>223</v>
-      </c>
-      <c r="L9" s="146" t="s">
-        <v>240</v>
+      <c r="K9" s="142" t="s">
+        <v>216</v>
+      </c>
+      <c r="L9" s="144" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B10" s="140" t="s">
-        <v>214</v>
+      <c r="B10" s="138" t="s">
+        <v>207</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
-      <c r="F10" s="148" t="s">
-        <v>243</v>
-      </c>
-      <c r="G10" s="141" t="s">
+      <c r="F10" s="146" t="s">
+        <v>236</v>
+      </c>
+      <c r="G10" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="134">
+      <c r="H10" s="132">
         <v>16</v>
       </c>
-      <c r="I10" s="134">
+      <c r="I10" s="132">
         <v>32</v>
       </c>
-      <c r="J10" s="134">
+      <c r="J10" s="132">
         <v>1</v>
       </c>
-      <c r="K10" s="144" t="s">
-        <v>213</v>
-      </c>
-      <c r="L10" s="146" t="s">
-        <v>242</v>
+      <c r="K10" s="142" t="s">
+        <v>206</v>
+      </c>
+      <c r="L10" s="144" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B11" s="140" t="s">
-        <v>216</v>
+      <c r="B11" s="138" t="s">
+        <v>209</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
-      <c r="F11" s="148" t="s">
-        <v>243</v>
-      </c>
-      <c r="G11" s="141" t="s">
+      <c r="F11" s="146" t="s">
+        <v>236</v>
+      </c>
+      <c r="G11" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="134">
+      <c r="H11" s="132">
         <v>16</v>
       </c>
-      <c r="I11" s="134">
+      <c r="I11" s="132">
         <v>32</v>
       </c>
-      <c r="J11" s="134">
+      <c r="J11" s="132">
         <v>1</v>
       </c>
-      <c r="K11" s="144" t="s">
-        <v>215</v>
-      </c>
-      <c r="L11" s="146" t="s">
-        <v>242</v>
+      <c r="K11" s="142" t="s">
+        <v>208</v>
+      </c>
+      <c r="L11" s="144" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B12" s="140" t="s">
-        <v>218</v>
+      <c r="B12" s="138" t="s">
+        <v>211</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
-      <c r="F12" s="148" t="s">
-        <v>243</v>
-      </c>
-      <c r="G12" s="141" t="s">
+      <c r="F12" s="146" t="s">
+        <v>236</v>
+      </c>
+      <c r="G12" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="134">
+      <c r="H12" s="132">
         <v>16</v>
       </c>
-      <c r="I12" s="134">
+      <c r="I12" s="132">
         <v>32</v>
       </c>
-      <c r="J12" s="134">
+      <c r="J12" s="132">
         <v>1</v>
       </c>
-      <c r="K12" s="144" t="s">
-        <v>217</v>
-      </c>
-      <c r="L12" s="146" t="s">
-        <v>242</v>
+      <c r="K12" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="L12" s="144" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B13" s="140" t="s">
-        <v>220</v>
+      <c r="B13" s="138" t="s">
+        <v>213</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="24"/>
       <c r="E13" s="24"/>
-      <c r="F13" s="148" t="s">
-        <v>244</v>
-      </c>
-      <c r="G13" s="141" t="s">
+      <c r="F13" s="146" t="s">
+        <v>237</v>
+      </c>
+      <c r="G13" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="134">
+      <c r="H13" s="132">
         <v>16</v>
       </c>
-      <c r="I13" s="134">
+      <c r="I13" s="132">
         <v>32</v>
       </c>
-      <c r="J13" s="134">
+      <c r="J13" s="132">
         <v>1</v>
       </c>
-      <c r="K13" s="144" t="s">
-        <v>219</v>
-      </c>
-      <c r="L13" s="146" t="s">
-        <v>242</v>
+      <c r="K13" s="142" t="s">
+        <v>212</v>
+      </c>
+      <c r="L13" s="144" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B14" s="140" t="s">
-        <v>225</v>
+      <c r="B14" s="138" t="s">
+        <v>218</v>
       </c>
       <c r="C14" s="63" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="68"/>
       <c r="E14" s="68"/>
-      <c r="F14" s="148" t="s">
-        <v>245</v>
-      </c>
-      <c r="G14" s="141" t="s">
+      <c r="F14" s="146" t="s">
+        <v>238</v>
+      </c>
+      <c r="G14" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="134">
+      <c r="H14" s="132">
         <v>16</v>
       </c>
-      <c r="I14" s="134">
+      <c r="I14" s="132">
         <v>32</v>
       </c>
-      <c r="J14" s="134">
+      <c r="J14" s="132">
         <v>1</v>
       </c>
-      <c r="K14" s="144" t="s">
-        <v>224</v>
-      </c>
-      <c r="L14" s="146" t="s">
-        <v>246</v>
+      <c r="K14" s="142" t="s">
+        <v>217</v>
+      </c>
+      <c r="L14" s="144" t="s">
+        <v>239</v>
       </c>
       <c r="M14" s="78"/>
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B15" s="140" t="s">
-        <v>227</v>
-      </c>
-      <c r="C15" s="134" t="s">
+      <c r="B15" s="138" t="s">
+        <v>220</v>
+      </c>
+      <c r="C15" s="132" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="68"/>
       <c r="E15" s="68"/>
-      <c r="F15" s="148" t="s">
-        <v>245</v>
-      </c>
-      <c r="G15" s="141" t="s">
+      <c r="F15" s="146" t="s">
+        <v>238</v>
+      </c>
+      <c r="G15" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="134">
+      <c r="H15" s="132">
         <v>16</v>
       </c>
-      <c r="I15" s="134">
+      <c r="I15" s="132">
         <v>32</v>
       </c>
-      <c r="J15" s="134">
+      <c r="J15" s="132">
         <v>1</v>
       </c>
-      <c r="K15" s="144" t="s">
-        <v>226</v>
-      </c>
-      <c r="L15" s="146" t="s">
-        <v>246</v>
+      <c r="K15" s="142" t="s">
+        <v>219</v>
+      </c>
+      <c r="L15" s="144" t="s">
+        <v>239</v>
       </c>
       <c r="M15" s="78"/>
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B16" s="140" t="s">
-        <v>229</v>
-      </c>
-      <c r="C16" s="134" t="s">
+      <c r="B16" s="138" t="s">
+        <v>222</v>
+      </c>
+      <c r="C16" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="147"/>
+      <c r="D16" s="145"/>
       <c r="E16" s="68"/>
-      <c r="F16" s="148" t="s">
-        <v>245</v>
-      </c>
-      <c r="G16" s="141" t="s">
+      <c r="F16" s="146" t="s">
+        <v>238</v>
+      </c>
+      <c r="G16" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="134">
+      <c r="H16" s="132">
         <v>16</v>
       </c>
-      <c r="I16" s="134">
+      <c r="I16" s="132">
         <v>32</v>
       </c>
-      <c r="J16" s="134">
+      <c r="J16" s="132">
         <v>1</v>
       </c>
-      <c r="K16" s="144" t="s">
-        <v>228</v>
-      </c>
-      <c r="L16" s="146" t="s">
-        <v>246</v>
+      <c r="K16" s="142" t="s">
+        <v>221</v>
+      </c>
+      <c r="L16" s="144" t="s">
+        <v>239</v>
       </c>
       <c r="M16" s="78"/>
     </row>
     <row r="17" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B17" s="140" t="s">
-        <v>231</v>
+      <c r="B17" s="138" t="s">
+        <v>224</v>
       </c>
       <c r="C17" s="68" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="68"/>
       <c r="E17" s="68"/>
-      <c r="F17" s="148" t="s">
-        <v>245</v>
-      </c>
-      <c r="G17" s="141" t="s">
+      <c r="F17" s="146" t="s">
+        <v>238</v>
+      </c>
+      <c r="G17" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="134">
+      <c r="H17" s="132">
         <v>16</v>
       </c>
-      <c r="I17" s="134">
+      <c r="I17" s="132">
         <v>32</v>
       </c>
-      <c r="J17" s="134">
+      <c r="J17" s="132">
         <v>1</v>
       </c>
-      <c r="K17" s="144" t="s">
-        <v>230</v>
-      </c>
-      <c r="L17" s="146" t="s">
-        <v>246</v>
+      <c r="K17" s="142" t="s">
+        <v>223</v>
+      </c>
+      <c r="L17" s="144" t="s">
+        <v>239</v>
       </c>
       <c r="M17" s="78"/>
     </row>
     <row r="18" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B18" s="140" t="s">
-        <v>233</v>
-      </c>
-      <c r="C18" s="134" t="s">
+      <c r="B18" s="138" t="s">
+        <v>226</v>
+      </c>
+      <c r="C18" s="132" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="68"/>
       <c r="E18" s="68"/>
-      <c r="F18" s="148" t="s">
-        <v>248</v>
-      </c>
-      <c r="G18" s="141" t="s">
+      <c r="F18" s="146" t="s">
+        <v>241</v>
+      </c>
+      <c r="G18" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="134">
+      <c r="H18" s="132">
         <v>16</v>
       </c>
-      <c r="I18" s="134">
+      <c r="I18" s="132">
         <v>32</v>
       </c>
-      <c r="J18" s="134">
+      <c r="J18" s="132">
         <v>1</v>
       </c>
-      <c r="K18" s="144" t="s">
-        <v>232</v>
-      </c>
-      <c r="L18" s="146" t="s">
-        <v>247</v>
+      <c r="K18" s="142" t="s">
+        <v>225</v>
+      </c>
+      <c r="L18" s="144" t="s">
+        <v>240</v>
       </c>
       <c r="M18" s="78"/>
-      <c r="N18" s="148"/>
+      <c r="N18" s="146"/>
     </row>
     <row r="19" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B19" s="140" t="s">
-        <v>235</v>
-      </c>
-      <c r="C19" s="134" t="s">
+      <c r="B19" s="138" t="s">
+        <v>228</v>
+      </c>
+      <c r="C19" s="132" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="68"/>
       <c r="E19" s="68"/>
-      <c r="F19" s="148" t="s">
-        <v>248</v>
-      </c>
-      <c r="G19" s="141" t="s">
+      <c r="F19" s="146" t="s">
+        <v>241</v>
+      </c>
+      <c r="G19" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="134">
+      <c r="H19" s="132">
         <v>16</v>
       </c>
-      <c r="I19" s="134">
+      <c r="I19" s="132">
         <v>32</v>
       </c>
-      <c r="J19" s="134">
+      <c r="J19" s="132">
         <v>1</v>
       </c>
-      <c r="K19" s="144" t="s">
-        <v>234</v>
-      </c>
-      <c r="L19" s="146" t="s">
-        <v>247</v>
+      <c r="K19" s="142" t="s">
+        <v>227</v>
+      </c>
+      <c r="L19" s="144" t="s">
+        <v>240</v>
       </c>
       <c r="M19" s="78"/>
     </row>
     <row r="20" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B20" s="140" t="s">
-        <v>239</v>
-      </c>
-      <c r="C20" s="134" t="s">
+      <c r="B20" s="138" t="s">
+        <v>232</v>
+      </c>
+      <c r="C20" s="132" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="68"/>
       <c r="E20" s="68"/>
-      <c r="F20" s="148" t="s">
-        <v>248</v>
-      </c>
-      <c r="G20" s="141" t="s">
+      <c r="F20" s="146" t="s">
+        <v>241</v>
+      </c>
+      <c r="G20" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="134">
+      <c r="H20" s="132">
         <v>16</v>
       </c>
-      <c r="I20" s="134">
+      <c r="I20" s="132">
         <v>32</v>
       </c>
-      <c r="J20" s="134">
+      <c r="J20" s="132">
         <v>1</v>
       </c>
-      <c r="K20" s="144" t="s">
-        <v>236</v>
-      </c>
-      <c r="L20" s="146" t="s">
-        <v>247</v>
+      <c r="K20" s="142" t="s">
+        <v>229</v>
+      </c>
+      <c r="L20" s="144" t="s">
+        <v>240</v>
       </c>
       <c r="M20" s="78"/>
     </row>
     <row r="21" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B21" s="140" t="s">
-        <v>238</v>
+      <c r="B21" s="138" t="s">
+        <v>231</v>
       </c>
       <c r="C21" s="68" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="68"/>
       <c r="E21" s="68"/>
-      <c r="F21" s="148" t="s">
-        <v>248</v>
-      </c>
-      <c r="G21" s="141" t="s">
+      <c r="F21" s="146" t="s">
+        <v>241</v>
+      </c>
+      <c r="G21" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="H21" s="134">
+      <c r="H21" s="132">
         <v>16</v>
       </c>
-      <c r="I21" s="134">
+      <c r="I21" s="132">
         <v>32</v>
       </c>
-      <c r="J21" s="134">
+      <c r="J21" s="132">
         <v>1</v>
       </c>
-      <c r="K21" s="144" t="s">
-        <v>237</v>
-      </c>
-      <c r="L21" s="146" t="s">
-        <v>247</v>
+      <c r="K21" s="142" t="s">
+        <v>230</v>
+      </c>
+      <c r="L21" s="144" t="s">
+        <v>240</v>
       </c>
       <c r="M21" s="78"/>
     </row>
     <row r="22" spans="2:14" ht="13.5" customHeight="1" thickBot="1">
       <c r="B22" s="79" t="s">
-        <v>202</v>
-      </c>
-      <c r="C22" s="137" t="s">
+        <v>195</v>
+      </c>
+      <c r="C22" s="135" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="80"/>
@@ -29563,8 +30438,8 @@
       <c r="H22" s="80"/>
       <c r="I22" s="80"/>
       <c r="J22" s="80"/>
-      <c r="K22" s="143"/>
-      <c r="L22" s="136"/>
+      <c r="K22" s="141"/>
+      <c r="L22" s="134"/>
       <c r="M22" s="78"/>
     </row>
     <row r="23" spans="2:14" ht="13.5" customHeight="1">
@@ -29576,7 +30451,7 @@
       <c r="C24" s="38"/>
       <c r="D24" s="38"/>
       <c r="E24" s="38"/>
-      <c r="F24" s="150"/>
+      <c r="F24" s="148"/>
     </row>
     <row r="25" spans="2:14" ht="13.5" customHeight="1">
       <c r="C25" s="38"/>
@@ -29594,7 +30469,7 @@
       <c r="E27" s="38"/>
     </row>
     <row r="28" spans="2:14" ht="13.5" customHeight="1">
-      <c r="F28" s="148"/>
+      <c r="F28" s="146"/>
     </row>
     <row r="29" spans="2:14" ht="13.5" customHeight="1">
       <c r="C29" s="38"/>

</xml_diff>

<commit_message>
cambios de fmod y sonido
cambios de nombres y reorganizacion rapida de tablas
</commit_message>
<xml_diff>
--- a/Tablas de sonido/Tabla_metadatos_no_lineal.xlsx
+++ b/Tablas de sonido/Tabla_metadatos_no_lineal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="495" windowWidth="21015" windowHeight="9405" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="495" windowWidth="21015" windowHeight="9405" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Principal" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="356">
   <si>
     <t>Tabla de metadatos - Música</t>
   </si>
@@ -1087,6 +1087,12 @@
   <si>
     <t>00:01:50</t>
   </si>
+  <si>
+    <t>SFX/Personaje Arpa golpea/golpe1</t>
+  </si>
+  <si>
+    <t>SFX/Personaje Guitarra golpea/golpe1</t>
+  </si>
 </sst>
 </file>
 
@@ -1550,7 +1556,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1800,14 +1806,8 @@
     <xf numFmtId="21" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="21" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3581,7 +3581,7 @@
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1">
       <c r="A4" s="12"/>
-      <c r="B4" s="129" t="s">
+      <c r="B4" s="127" t="s">
         <v>177</v>
       </c>
       <c r="C4" s="14"/>
@@ -6975,7 +6975,7 @@
       <c r="L3" s="11"/>
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B4" s="129" t="s">
+      <c r="B4" s="127" t="s">
         <v>177</v>
       </c>
       <c r="C4" s="14"/>
@@ -12451,8 +12451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -12556,7 +12556,7 @@
       <c r="L3" s="11"/>
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B4" s="129" t="s">
+      <c r="B4" s="127" t="s">
         <v>177</v>
       </c>
       <c r="C4" s="76"/>
@@ -12676,7 +12676,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="29" t="s">
         <v>115</v>
       </c>
       <c r="C8" s="14"/>
@@ -12710,86 +12710,58 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B9" s="13" t="s">
-        <v>117</v>
+      <c r="B9" s="29" t="s">
+        <v>354</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
       <c r="E9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="56" t="s">
-        <v>90</v>
-      </c>
-      <c r="H9" s="65">
-        <v>22.05</v>
-      </c>
-      <c r="I9" s="56">
-        <v>24</v>
-      </c>
-      <c r="J9" s="56" t="s">
-        <v>62</v>
-      </c>
-      <c r="K9" s="89">
-        <v>3.9675925925925927E-2</v>
-      </c>
-      <c r="L9" s="91" t="s">
-        <v>118</v>
-      </c>
+      <c r="F9" s="117"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="89"/>
+      <c r="L9" s="91"/>
       <c r="N9" s="27" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B10" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25" t="s">
+      <c r="B10" s="29" t="s">
+        <v>355</v>
+      </c>
+      <c r="C10" s="122"/>
+      <c r="D10" s="122"/>
+      <c r="E10" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="60" t="s">
-        <v>79</v>
-      </c>
-      <c r="G10" s="56" t="s">
-        <v>90</v>
-      </c>
-      <c r="H10" s="65">
-        <v>22.05</v>
-      </c>
-      <c r="I10" s="56">
-        <v>24</v>
-      </c>
-      <c r="J10" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="K10" s="89">
-        <v>4.7453703703703704E-4</v>
-      </c>
-      <c r="L10" s="91" t="s">
-        <v>120</v>
-      </c>
+      <c r="F10" s="117"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="89"/>
+      <c r="L10" s="91"/>
       <c r="N10" s="27" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B11" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="25" t="s">
+      <c r="B11" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="122"/>
+      <c r="D11" s="122"/>
+      <c r="E11" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="G11" s="55" t="s">
+      <c r="F11" s="117" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="56" t="s">
         <v>90</v>
       </c>
       <c r="H11" s="65">
@@ -12798,32 +12770,32 @@
       <c r="I11" s="56">
         <v>24</v>
       </c>
-      <c r="J11" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" s="66">
-        <v>8.0439814814814818E-3</v>
-      </c>
-      <c r="L11" s="72" t="s">
-        <v>122</v>
+      <c r="J11" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11" s="89">
+        <v>3.9675925925925927E-2</v>
+      </c>
+      <c r="L11" s="91" t="s">
+        <v>118</v>
       </c>
       <c r="N11" s="27" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B12" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15" t="s">
+      <c r="B12" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="60" t="s">
+      <c r="F12" s="117" t="s">
         <v>79</v>
       </c>
-      <c r="G12" s="55" t="s">
+      <c r="G12" s="56" t="s">
         <v>90</v>
       </c>
       <c r="H12" s="65">
@@ -12832,32 +12804,32 @@
       <c r="I12" s="56">
         <v>24</v>
       </c>
-      <c r="J12" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="K12" s="66">
-        <v>3.7615740740740739E-3</v>
+      <c r="J12" s="65" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="89">
+        <v>4.7453703703703704E-4</v>
       </c>
       <c r="L12" s="91" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="N12" s="27" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B13" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="15" t="s">
+      <c r="B13" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="60" t="s">
+      <c r="F13" s="117" t="s">
         <v>89</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="G13" s="65" t="s">
         <v>90</v>
       </c>
       <c r="H13" s="65">
@@ -12866,32 +12838,32 @@
       <c r="I13" s="56">
         <v>24</v>
       </c>
-      <c r="J13" s="21" t="s">
+      <c r="J13" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="89">
-        <v>6.8287037037037036E-4</v>
-      </c>
-      <c r="L13" s="91" t="s">
-        <v>126</v>
+      <c r="K13" s="92">
+        <v>8.0439814814814818E-3</v>
+      </c>
+      <c r="L13" s="72" t="s">
+        <v>122</v>
       </c>
       <c r="N13" s="27" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B14" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="15" t="s">
+      <c r="B14" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" s="122"/>
+      <c r="D14" s="122"/>
+      <c r="E14" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="G14" s="21" t="s">
+      <c r="F14" s="117" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="65" t="s">
         <v>90</v>
       </c>
       <c r="H14" s="65">
@@ -12900,359 +12872,416 @@
       <c r="I14" s="56">
         <v>24</v>
       </c>
-      <c r="J14" s="21" t="s">
+      <c r="J14" s="65" t="s">
         <v>62</v>
       </c>
       <c r="K14" s="92">
-        <v>5.3819444444444444E-3</v>
-      </c>
-      <c r="L14" s="90" t="s">
-        <v>128</v>
+        <v>3.7615740740740739E-3</v>
+      </c>
+      <c r="L14" s="91" t="s">
+        <v>124</v>
       </c>
       <c r="N14" s="27" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="122"/>
+      <c r="D15" s="122"/>
+      <c r="E15" s="122" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="117" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="H15" s="65">
+        <v>22.05</v>
+      </c>
+      <c r="I15" s="56">
+        <v>24</v>
+      </c>
+      <c r="J15" s="65" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="89">
+        <v>6.8287037037037036E-4</v>
+      </c>
+      <c r="L15" s="91" t="s">
+        <v>126</v>
+      </c>
+      <c r="N15" s="27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="13.5" customHeight="1">
+      <c r="B16" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="122" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="117" t="s">
+        <v>89</v>
+      </c>
+      <c r="G16" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" s="65">
+        <v>22.05</v>
+      </c>
+      <c r="I16" s="56">
+        <v>24</v>
+      </c>
+      <c r="J16" s="65" t="s">
+        <v>62</v>
+      </c>
+      <c r="K16" s="92">
+        <v>5.3819444444444444E-3</v>
+      </c>
+      <c r="L16" s="90" t="s">
+        <v>128</v>
+      </c>
+      <c r="N16" s="27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" ht="13.5" customHeight="1">
+      <c r="B17" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25" t="s">
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="60" t="s">
+      <c r="F17" s="117" t="s">
         <v>79</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G17" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="21">
-        <v>16</v>
-      </c>
-      <c r="I15" s="21">
-        <v>32</v>
-      </c>
-      <c r="J15" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="K15" s="92">
-        <v>6.6666666666666671E-3</v>
-      </c>
-      <c r="L15" s="90" t="s">
-        <v>130</v>
-      </c>
-      <c r="N15" s="27" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B16" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="21">
-        <v>16</v>
-      </c>
-      <c r="I16" s="65">
-        <v>32</v>
-      </c>
-      <c r="J16" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="K16" s="66">
-        <v>1.5277777777777779E-3</v>
-      </c>
-      <c r="L16" s="90" t="s">
-        <v>133</v>
-      </c>
-      <c r="N16" s="27" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B17" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="21">
+      <c r="H17" s="65">
         <v>16</v>
       </c>
       <c r="I17" s="65">
         <v>32</v>
       </c>
-      <c r="J17" s="21" t="s">
+      <c r="J17" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="K17" s="66">
-        <v>1.8865740740740742E-3</v>
-      </c>
-      <c r="L17" s="91" t="s">
-        <v>135</v>
+      <c r="K17" s="92">
+        <v>6.6666666666666671E-3</v>
+      </c>
+      <c r="L17" s="90" t="s">
+        <v>130</v>
       </c>
       <c r="N17" s="27" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="18" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B18" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15" t="s">
+      <c r="B18" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="G18" s="21" t="s">
+      <c r="F18" s="117" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="21">
+      <c r="H18" s="65">
         <v>16</v>
       </c>
       <c r="I18" s="65">
         <v>32</v>
       </c>
-      <c r="J18" s="21" t="s">
+      <c r="J18" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="K18" s="66">
-        <v>7.5231481481481482E-4</v>
-      </c>
-      <c r="L18" s="91" t="s">
-        <v>137</v>
+      <c r="K18" s="92">
+        <v>1.5277777777777779E-3</v>
+      </c>
+      <c r="L18" s="90" t="s">
+        <v>133</v>
       </c>
       <c r="N18" s="27" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="19" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B19" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15" t="s">
+      <c r="B19" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="C19" s="122"/>
+      <c r="D19" s="122"/>
+      <c r="E19" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="60" t="s">
-        <v>79</v>
-      </c>
-      <c r="G19" s="21" t="s">
+      <c r="F19" s="117" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="21">
+      <c r="H19" s="65">
         <v>16</v>
       </c>
-      <c r="I19" s="21">
+      <c r="I19" s="65">
         <v>32</v>
       </c>
-      <c r="J19" s="21" t="s">
-        <v>62</v>
+      <c r="J19" s="65" t="s">
+        <v>20</v>
       </c>
       <c r="K19" s="92">
-        <v>1.2037037037037038E-3</v>
+        <v>1.8865740740740742E-3</v>
       </c>
       <c r="L19" s="91" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="N19" s="27" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="20" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="C20" s="122"/>
+      <c r="D20" s="122"/>
+      <c r="E20" s="122" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="117" t="s">
+        <v>89</v>
+      </c>
+      <c r="G20" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="65">
+        <v>16</v>
+      </c>
+      <c r="I20" s="65">
+        <v>32</v>
+      </c>
+      <c r="J20" s="65" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20" s="92">
+        <v>7.5231481481481482E-4</v>
+      </c>
+      <c r="L20" s="91" t="s">
+        <v>137</v>
+      </c>
+      <c r="N20" s="27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" ht="13.5" customHeight="1">
+      <c r="B21" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="C21" s="122"/>
+      <c r="D21" s="122"/>
+      <c r="E21" s="122" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="117" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="65">
+        <v>16</v>
+      </c>
+      <c r="I21" s="65">
+        <v>32</v>
+      </c>
+      <c r="J21" s="65" t="s">
+        <v>62</v>
+      </c>
+      <c r="K21" s="92">
+        <v>1.2037037037037038E-3</v>
+      </c>
+      <c r="L21" s="91" t="s">
+        <v>139</v>
+      </c>
+      <c r="N21" s="27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" ht="13.5" customHeight="1">
+      <c r="B22" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25" t="s">
+      <c r="C22" s="70"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="60" t="s">
+      <c r="F22" s="117" t="s">
         <v>54</v>
       </c>
-      <c r="G20" s="55" t="s">
+      <c r="G22" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="H20" s="65">
+      <c r="H22" s="65">
         <v>22.05</v>
       </c>
-      <c r="I20" s="55">
+      <c r="I22" s="65">
         <v>24</v>
       </c>
-      <c r="J20" s="21" t="s">
+      <c r="J22" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="K20" s="93">
+      <c r="K22" s="92">
         <v>3.6805555555555554E-3</v>
       </c>
-      <c r="L20" s="91" t="s">
+      <c r="L22" s="91" t="s">
         <v>141</v>
       </c>
-      <c r="N20" s="27" t="s">
+      <c r="N22" s="27" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B21" s="13" t="s">
+    <row r="23" spans="2:14" ht="13.5" customHeight="1">
+      <c r="B23" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="25" t="s">
+      <c r="C23" s="70"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="60" t="s">
+      <c r="F23" s="117" t="s">
         <v>54</v>
       </c>
-      <c r="G21" s="55" t="s">
+      <c r="G23" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="H21" s="65">
+      <c r="H23" s="65">
         <v>22.05</v>
       </c>
-      <c r="I21" s="55">
+      <c r="I23" s="65">
         <v>24</v>
       </c>
-      <c r="J21" s="21" t="s">
+      <c r="J23" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="K21" s="66">
+      <c r="K23" s="92">
         <v>3.6805555555555554E-3</v>
       </c>
-      <c r="L21" s="91" t="s">
+      <c r="L23" s="91" t="s">
         <v>141</v>
       </c>
-      <c r="N21" s="27" t="s">
+      <c r="N23" s="27" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B22" s="13" t="s">
+    <row r="24" spans="2:14" ht="13.5" customHeight="1">
+      <c r="B24" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="15" t="s">
+      <c r="C24" s="122"/>
+      <c r="D24" s="122"/>
+      <c r="E24" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="60" t="s">
+      <c r="F24" s="117" t="s">
         <v>54</v>
       </c>
-      <c r="G22" s="21" t="s">
+      <c r="G24" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="65">
+      <c r="H24" s="65">
         <v>16</v>
       </c>
-      <c r="I22" s="65">
+      <c r="I24" s="65">
         <v>32</v>
       </c>
-      <c r="J22" s="21" t="s">
+      <c r="J24" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="K22" s="93">
+      <c r="K24" s="92">
         <v>5.5439814814814813E-3</v>
       </c>
-      <c r="L22" s="72" t="s">
+      <c r="L24" s="72" t="s">
         <v>144</v>
       </c>
-      <c r="N22" s="27" t="s">
+      <c r="N24" s="27" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B23" s="30" t="s">
+    <row r="25" spans="2:14" ht="13.5" customHeight="1" thickBot="1">
+      <c r="B25" s="79" t="s">
         <v>145</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="32" t="s">
+      <c r="C25" s="125"/>
+      <c r="D25" s="125"/>
+      <c r="E25" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="94" t="s">
+      <c r="F25" s="93" t="s">
         <v>79</v>
       </c>
-      <c r="G23" s="95" t="s">
+      <c r="G25" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="H23" s="96">
+      <c r="H25" s="94">
         <v>16</v>
       </c>
-      <c r="I23" s="96">
+      <c r="I25" s="94">
         <v>32</v>
       </c>
-      <c r="J23" s="95" t="s">
+      <c r="J25" s="94" t="s">
         <v>62</v>
       </c>
-      <c r="K23" s="97">
+      <c r="K25" s="95">
         <v>3.5185185185185185E-3</v>
       </c>
-      <c r="L23" s="98" t="s">
+      <c r="L25" s="96" t="s">
         <v>146</v>
       </c>
-      <c r="N23" s="27" t="s">
+      <c r="N25" s="27" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B24" s="99"/>
-      <c r="C24" s="38">
-        <f t="shared" ref="C24:E24" si="0">COUNTA(C4:C23)</f>
+    <row r="26" spans="2:14" ht="13.5" customHeight="1">
+      <c r="B26" s="97"/>
+      <c r="C26" s="38">
+        <f t="shared" ref="C26:I26" si="0">COUNTA(C6:C25)</f>
         <v>0</v>
       </c>
-      <c r="D24" s="38">
+      <c r="D26" s="38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E24" s="38">
+      <c r="E26" s="38">
         <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B25" s="99"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-    </row>
-    <row r="26" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B26" s="99"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
+        <v>20</v>
+      </c>
     </row>
     <row r="27" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B27" s="99"/>
+      <c r="B27" s="97"/>
       <c r="C27" s="38"/>
       <c r="D27" s="38"/>
       <c r="E27" s="38"/>
     </row>
     <row r="28" spans="2:14" ht="13.5" customHeight="1">
+      <c r="B28" s="97"/>
       <c r="C28" s="38"/>
       <c r="D28" s="38"/>
       <c r="E28" s="38"/>
@@ -18114,7 +18143,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -18122,7 +18151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1030"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
@@ -18220,7 +18249,7 @@
       <c r="L3" s="11"/>
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B4" s="129" t="s">
+      <c r="B4" s="127" t="s">
         <v>177</v>
       </c>
       <c r="C4" s="15"/>
@@ -18241,18 +18270,18 @@
       <c r="B5" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="124" t="s">
+      <c r="C5" s="122" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="70"/>
       <c r="E5" s="70"/>
-      <c r="F5" s="138" t="s">
+      <c r="F5" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G5" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H5" s="146">
+      <c r="H5" s="144">
         <v>22.05</v>
       </c>
       <c r="I5" s="70">
@@ -18261,10 +18290,10 @@
       <c r="J5" s="70">
         <v>1</v>
       </c>
-      <c r="K5" s="141" t="s">
+      <c r="K5" s="139" t="s">
         <v>226</v>
       </c>
-      <c r="L5" s="143" t="s">
+      <c r="L5" s="141" t="s">
         <v>227</v>
       </c>
       <c r="N5" s="27" t="s">
@@ -18275,18 +18304,18 @@
       <c r="B6" s="29" t="s">
         <v>224</v>
       </c>
-      <c r="C6" s="124" t="s">
+      <c r="C6" s="122" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="70"/>
       <c r="E6" s="70"/>
-      <c r="F6" s="138" t="s">
+      <c r="F6" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G6" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H6" s="146">
+      <c r="H6" s="144">
         <v>22.05</v>
       </c>
       <c r="I6" s="70">
@@ -18295,10 +18324,10 @@
       <c r="J6" s="70">
         <v>1</v>
       </c>
-      <c r="K6" s="147" t="s">
+      <c r="K6" s="145" t="s">
         <v>353</v>
       </c>
-      <c r="L6" s="145" t="s">
+      <c r="L6" s="143" t="s">
         <v>228</v>
       </c>
       <c r="N6" s="27"/>
@@ -18307,18 +18336,18 @@
       <c r="B7" s="29" t="s">
         <v>225</v>
       </c>
-      <c r="C7" s="124" t="s">
+      <c r="C7" s="122" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="70"/>
       <c r="E7" s="70"/>
-      <c r="F7" s="138" t="s">
+      <c r="F7" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G7" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H7" s="146">
+      <c r="H7" s="144">
         <v>22.05</v>
       </c>
       <c r="I7" s="70">
@@ -18327,10 +18356,10 @@
       <c r="J7" s="70">
         <v>1</v>
       </c>
-      <c r="K7" s="141" t="s">
+      <c r="K7" s="139" t="s">
         <v>229</v>
       </c>
-      <c r="L7" s="145" t="s">
+      <c r="L7" s="143" t="s">
         <v>230</v>
       </c>
       <c r="N7" s="27" t="s">
@@ -18346,13 +18375,13 @@
       </c>
       <c r="D8" s="24"/>
       <c r="E8" s="24"/>
-      <c r="F8" s="138" t="s">
+      <c r="F8" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G8" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H8" s="146">
+      <c r="H8" s="144">
         <v>22.05</v>
       </c>
       <c r="I8" s="70">
@@ -18361,10 +18390,10 @@
       <c r="J8" s="70">
         <v>1</v>
       </c>
-      <c r="K8" s="141" t="s">
+      <c r="K8" s="139" t="s">
         <v>231</v>
       </c>
-      <c r="L8" s="145" t="s">
+      <c r="L8" s="143" t="s">
         <v>232</v>
       </c>
       <c r="N8" s="27" t="s">
@@ -18372,21 +18401,21 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B9" s="128" t="s">
+      <c r="B9" s="126" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="124" t="s">
+      <c r="C9" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="124"/>
-      <c r="E9" s="124"/>
-      <c r="F9" s="138" t="s">
+      <c r="D9" s="122"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G9" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H9" s="146">
+      <c r="H9" s="144">
         <v>22.05</v>
       </c>
       <c r="I9" s="70">
@@ -18395,30 +18424,30 @@
       <c r="J9" s="70">
         <v>1</v>
       </c>
-      <c r="K9" s="141" t="s">
+      <c r="K9" s="139" t="s">
         <v>234</v>
       </c>
-      <c r="L9" s="145" t="s">
+      <c r="L9" s="143" t="s">
         <v>235</v>
       </c>
       <c r="N9" s="27"/>
     </row>
     <row r="10" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B10" s="128" t="s">
+      <c r="B10" s="126" t="s">
         <v>233</v>
       </c>
-      <c r="C10" s="124" t="s">
+      <c r="C10" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="124"/>
-      <c r="E10" s="124"/>
-      <c r="F10" s="138" t="s">
+      <c r="D10" s="122"/>
+      <c r="E10" s="122"/>
+      <c r="F10" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G10" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H10" s="146">
+      <c r="H10" s="144">
         <v>22.05</v>
       </c>
       <c r="I10" s="70">
@@ -18427,10 +18456,10 @@
       <c r="J10" s="70">
         <v>1</v>
       </c>
-      <c r="K10" s="141" t="s">
+      <c r="K10" s="139" t="s">
         <v>236</v>
       </c>
-      <c r="L10" s="145" t="s">
+      <c r="L10" s="143" t="s">
         <v>237</v>
       </c>
       <c r="N10" s="27" t="s">
@@ -18441,18 +18470,18 @@
       <c r="B11" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="124" t="s">
+      <c r="C11" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="124"/>
-      <c r="E11" s="124"/>
-      <c r="F11" s="138" t="s">
+      <c r="D11" s="122"/>
+      <c r="E11" s="122"/>
+      <c r="F11" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G11" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H11" s="146">
+      <c r="H11" s="144">
         <v>22.05</v>
       </c>
       <c r="I11" s="70">
@@ -18461,10 +18490,10 @@
       <c r="J11" s="70">
         <v>1</v>
       </c>
-      <c r="K11" s="141" t="s">
+      <c r="K11" s="139" t="s">
         <v>242</v>
       </c>
-      <c r="L11" s="145" t="s">
+      <c r="L11" s="143" t="s">
         <v>243</v>
       </c>
       <c r="N11" s="27" t="s">
@@ -18472,21 +18501,21 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B12" s="128" t="s">
+      <c r="B12" s="126" t="s">
         <v>238</v>
       </c>
-      <c r="C12" s="124" t="s">
+      <c r="C12" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="124"/>
-      <c r="E12" s="124"/>
-      <c r="F12" s="138" t="s">
+      <c r="D12" s="122"/>
+      <c r="E12" s="122"/>
+      <c r="F12" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G12" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H12" s="146">
+      <c r="H12" s="144">
         <v>22.05</v>
       </c>
       <c r="I12" s="70">
@@ -18495,10 +18524,10 @@
       <c r="J12" s="70">
         <v>1</v>
       </c>
-      <c r="K12" s="141" t="s">
+      <c r="K12" s="139" t="s">
         <v>244</v>
       </c>
-      <c r="L12" s="145" t="s">
+      <c r="L12" s="143" t="s">
         <v>245</v>
       </c>
       <c r="N12" s="27" t="s">
@@ -18506,21 +18535,21 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B13" s="128" t="s">
+      <c r="B13" s="126" t="s">
         <v>239</v>
       </c>
-      <c r="C13" s="124" t="s">
+      <c r="C13" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="124"/>
-      <c r="E13" s="124"/>
-      <c r="F13" s="138" t="s">
+      <c r="D13" s="122"/>
+      <c r="E13" s="122"/>
+      <c r="F13" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G13" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H13" s="146">
+      <c r="H13" s="144">
         <v>22.05</v>
       </c>
       <c r="I13" s="70">
@@ -18529,10 +18558,10 @@
       <c r="J13" s="70">
         <v>1</v>
       </c>
-      <c r="K13" s="141" t="s">
+      <c r="K13" s="139" t="s">
         <v>246</v>
       </c>
-      <c r="L13" s="145" t="s">
+      <c r="L13" s="143" t="s">
         <v>247</v>
       </c>
       <c r="M13" s="78"/>
@@ -18541,21 +18570,21 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B14" s="128" t="s">
+      <c r="B14" s="126" t="s">
         <v>240</v>
       </c>
-      <c r="C14" s="124" t="s">
+      <c r="C14" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="124"/>
-      <c r="E14" s="124"/>
-      <c r="F14" s="138" t="s">
+      <c r="D14" s="122"/>
+      <c r="E14" s="122"/>
+      <c r="F14" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G14" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H14" s="146">
+      <c r="H14" s="144">
         <v>22.05</v>
       </c>
       <c r="I14" s="70">
@@ -18564,10 +18593,10 @@
       <c r="J14" s="70">
         <v>1</v>
       </c>
-      <c r="K14" s="147" t="s">
+      <c r="K14" s="145" t="s">
         <v>231</v>
       </c>
-      <c r="L14" s="145" t="s">
+      <c r="L14" s="143" t="s">
         <v>248</v>
       </c>
       <c r="M14" s="78"/>
@@ -18576,21 +18605,21 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B15" s="128" t="s">
+      <c r="B15" s="126" t="s">
         <v>241</v>
       </c>
-      <c r="C15" s="124" t="s">
+      <c r="C15" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="124"/>
-      <c r="E15" s="124"/>
-      <c r="F15" s="138" t="s">
+      <c r="D15" s="122"/>
+      <c r="E15" s="122"/>
+      <c r="F15" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G15" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H15" s="146">
+      <c r="H15" s="144">
         <v>22.05</v>
       </c>
       <c r="I15" s="70">
@@ -18599,10 +18628,10 @@
       <c r="J15" s="70">
         <v>1</v>
       </c>
-      <c r="K15" s="148" t="s">
+      <c r="K15" s="146" t="s">
         <v>249</v>
       </c>
-      <c r="L15" s="145" t="s">
+      <c r="L15" s="143" t="s">
         <v>250</v>
       </c>
       <c r="N15" s="27" t="s">
@@ -18610,7 +18639,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B16" s="128" t="s">
+      <c r="B16" s="126" t="s">
         <v>251</v>
       </c>
       <c r="C16" s="15" t="s">
@@ -18618,13 +18647,13 @@
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
-      <c r="F16" s="138" t="s">
+      <c r="F16" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G16" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H16" s="146">
+      <c r="H16" s="144">
         <v>22.05</v>
       </c>
       <c r="I16" s="70">
@@ -18633,10 +18662,10 @@
       <c r="J16" s="70">
         <v>1</v>
       </c>
-      <c r="K16" s="148" t="s">
+      <c r="K16" s="146" t="s">
         <v>253</v>
       </c>
-      <c r="L16" s="145" t="s">
+      <c r="L16" s="143" t="s">
         <v>254</v>
       </c>
       <c r="N16" s="27" t="s">
@@ -18644,7 +18673,7 @@
       </c>
     </row>
     <row r="17" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B17" s="128" t="s">
+      <c r="B17" s="126" t="s">
         <v>252</v>
       </c>
       <c r="C17" s="15" t="s">
@@ -18652,13 +18681,13 @@
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
-      <c r="F17" s="138" t="s">
+      <c r="F17" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G17" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H17" s="146">
+      <c r="H17" s="144">
         <v>22.05</v>
       </c>
       <c r="I17" s="70">
@@ -18667,10 +18696,10 @@
       <c r="J17" s="70">
         <v>1</v>
       </c>
-      <c r="K17" s="148" t="s">
+      <c r="K17" s="146" t="s">
         <v>255</v>
       </c>
-      <c r="L17" s="145" t="s">
+      <c r="L17" s="143" t="s">
         <v>256</v>
       </c>
       <c r="N17" s="27" t="s">
@@ -18681,18 +18710,18 @@
       <c r="B18" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="124" t="s">
+      <c r="C18" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="124"/>
-      <c r="E18" s="124"/>
-      <c r="F18" s="138" t="s">
+      <c r="D18" s="122"/>
+      <c r="E18" s="122"/>
+      <c r="F18" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G18" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H18" s="146">
+      <c r="H18" s="144">
         <v>22.05</v>
       </c>
       <c r="I18" s="70">
@@ -18701,10 +18730,10 @@
       <c r="J18" s="70">
         <v>1</v>
       </c>
-      <c r="K18" s="148" t="s">
+      <c r="K18" s="146" t="s">
         <v>263</v>
       </c>
-      <c r="L18" s="145" t="s">
+      <c r="L18" s="143" t="s">
         <v>264</v>
       </c>
       <c r="N18" s="27" t="s">
@@ -18712,21 +18741,21 @@
       </c>
     </row>
     <row r="19" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B19" s="128" t="s">
+      <c r="B19" s="126" t="s">
         <v>257</v>
       </c>
-      <c r="C19" s="124" t="s">
+      <c r="C19" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="124"/>
-      <c r="E19" s="124"/>
-      <c r="F19" s="138" t="s">
+      <c r="D19" s="122"/>
+      <c r="E19" s="122"/>
+      <c r="F19" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G19" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H19" s="146">
+      <c r="H19" s="144">
         <v>22.05</v>
       </c>
       <c r="I19" s="70">
@@ -18735,10 +18764,10 @@
       <c r="J19" s="70">
         <v>1</v>
       </c>
-      <c r="K19" s="148" t="s">
+      <c r="K19" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="L19" s="145" t="s">
+      <c r="L19" s="143" t="s">
         <v>266</v>
       </c>
       <c r="N19" s="27" t="s">
@@ -18746,21 +18775,21 @@
       </c>
     </row>
     <row r="20" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B20" s="128" t="s">
+      <c r="B20" s="126" t="s">
         <v>258</v>
       </c>
-      <c r="C20" s="124" t="s">
+      <c r="C20" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="124"/>
-      <c r="E20" s="124"/>
-      <c r="F20" s="138" t="s">
+      <c r="D20" s="122"/>
+      <c r="E20" s="122"/>
+      <c r="F20" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G20" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H20" s="146">
+      <c r="H20" s="144">
         <v>22.05</v>
       </c>
       <c r="I20" s="70">
@@ -18769,10 +18798,10 @@
       <c r="J20" s="70">
         <v>1</v>
       </c>
-      <c r="K20" s="148" t="s">
+      <c r="K20" s="146" t="s">
         <v>267</v>
       </c>
-      <c r="L20" s="145" t="s">
+      <c r="L20" s="143" t="s">
         <v>268</v>
       </c>
       <c r="N20" s="27" t="s">
@@ -18780,21 +18809,21 @@
       </c>
     </row>
     <row r="21" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B21" s="128" t="s">
+      <c r="B21" s="126" t="s">
         <v>259</v>
       </c>
-      <c r="C21" s="124" t="s">
+      <c r="C21" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="124"/>
-      <c r="E21" s="124"/>
-      <c r="F21" s="138" t="s">
+      <c r="D21" s="122"/>
+      <c r="E21" s="122"/>
+      <c r="F21" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G21" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H21" s="146">
+      <c r="H21" s="144">
         <v>22.05</v>
       </c>
       <c r="I21" s="70">
@@ -18803,10 +18832,10 @@
       <c r="J21" s="70">
         <v>1</v>
       </c>
-      <c r="K21" s="148" t="s">
+      <c r="K21" s="146" t="s">
         <v>269</v>
       </c>
-      <c r="L21" s="145" t="s">
+      <c r="L21" s="143" t="s">
         <v>270</v>
       </c>
       <c r="N21" s="27" t="s">
@@ -18814,21 +18843,21 @@
       </c>
     </row>
     <row r="22" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B22" s="128" t="s">
+      <c r="B22" s="126" t="s">
         <v>260</v>
       </c>
-      <c r="C22" s="124" t="s">
+      <c r="C22" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="124"/>
-      <c r="E22" s="124"/>
-      <c r="F22" s="138" t="s">
+      <c r="D22" s="122"/>
+      <c r="E22" s="122"/>
+      <c r="F22" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G22" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H22" s="146">
+      <c r="H22" s="144">
         <v>22.05</v>
       </c>
       <c r="I22" s="70">
@@ -18837,30 +18866,30 @@
       <c r="J22" s="70">
         <v>1</v>
       </c>
-      <c r="K22" s="148" t="s">
+      <c r="K22" s="146" t="s">
         <v>271</v>
       </c>
-      <c r="L22" s="145" t="s">
+      <c r="L22" s="143" t="s">
         <v>272</v>
       </c>
       <c r="N22" s="27"/>
     </row>
     <row r="23" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B23" s="128" t="s">
+      <c r="B23" s="126" t="s">
         <v>261</v>
       </c>
-      <c r="C23" s="124" t="s">
+      <c r="C23" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="124"/>
-      <c r="E23" s="124"/>
-      <c r="F23" s="138" t="s">
+      <c r="D23" s="122"/>
+      <c r="E23" s="122"/>
+      <c r="F23" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G23" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H23" s="146">
+      <c r="H23" s="144">
         <v>22.05</v>
       </c>
       <c r="I23" s="70">
@@ -18869,16 +18898,16 @@
       <c r="J23" s="70">
         <v>1</v>
       </c>
-      <c r="K23" s="148" t="s">
+      <c r="K23" s="146" t="s">
         <v>273</v>
       </c>
-      <c r="L23" s="145" t="s">
+      <c r="L23" s="143" t="s">
         <v>274</v>
       </c>
       <c r="N23" s="27"/>
     </row>
     <row r="24" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B24" s="128" t="s">
+      <c r="B24" s="126" t="s">
         <v>262</v>
       </c>
       <c r="C24" s="15" t="s">
@@ -18886,13 +18915,13 @@
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
-      <c r="F24" s="138" t="s">
+      <c r="F24" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G24" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H24" s="146">
+      <c r="H24" s="144">
         <v>22.05</v>
       </c>
       <c r="I24" s="70">
@@ -18901,10 +18930,10 @@
       <c r="J24" s="70">
         <v>1</v>
       </c>
-      <c r="K24" s="148" t="s">
+      <c r="K24" s="146" t="s">
         <v>275</v>
       </c>
-      <c r="L24" s="145" t="s">
+      <c r="L24" s="143" t="s">
         <v>276</v>
       </c>
       <c r="N24" s="27" t="s">
@@ -18920,13 +18949,13 @@
       </c>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
-      <c r="F25" s="138"/>
+      <c r="F25" s="136"/>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
-      <c r="K25" s="147"/>
-      <c r="L25" s="144"/>
+      <c r="K25" s="145"/>
+      <c r="L25" s="142"/>
       <c r="N25" s="27" t="s">
         <v>93</v>
       </c>
@@ -18940,13 +18969,13 @@
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
-      <c r="F26" s="138"/>
+      <c r="F26" s="136"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
-      <c r="K26" s="147"/>
-      <c r="L26" s="144"/>
+      <c r="K26" s="145"/>
+      <c r="L26" s="142"/>
       <c r="N26" s="27" t="s">
         <v>93</v>
       </c>
@@ -18955,18 +18984,18 @@
       <c r="B27" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="C27" s="124" t="s">
+      <c r="C27" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="124"/>
-      <c r="E27" s="124"/>
-      <c r="F27" s="138" t="s">
+      <c r="D27" s="122"/>
+      <c r="E27" s="122"/>
+      <c r="F27" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G27" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H27" s="146">
+      <c r="H27" s="144">
         <v>22.05</v>
       </c>
       <c r="I27" s="70">
@@ -18975,10 +19004,10 @@
       <c r="J27" s="70">
         <v>1</v>
       </c>
-      <c r="K27" s="148" t="s">
+      <c r="K27" s="146" t="s">
         <v>281</v>
       </c>
-      <c r="L27" s="145" t="s">
+      <c r="L27" s="143" t="s">
         <v>282</v>
       </c>
       <c r="M27" s="78"/>
@@ -18987,21 +19016,21 @@
       </c>
     </row>
     <row r="28" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B28" s="128" t="s">
+      <c r="B28" s="126" t="s">
         <v>277</v>
       </c>
-      <c r="C28" s="124" t="s">
+      <c r="C28" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="124"/>
-      <c r="E28" s="124"/>
-      <c r="F28" s="138" t="s">
+      <c r="D28" s="122"/>
+      <c r="E28" s="122"/>
+      <c r="F28" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G28" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H28" s="146">
+      <c r="H28" s="144">
         <v>22.05</v>
       </c>
       <c r="I28" s="70">
@@ -19010,10 +19039,10 @@
       <c r="J28" s="70">
         <v>1</v>
       </c>
-      <c r="K28" s="148" t="s">
+      <c r="K28" s="146" t="s">
         <v>283</v>
       </c>
-      <c r="L28" s="145" t="s">
+      <c r="L28" s="143" t="s">
         <v>284</v>
       </c>
       <c r="M28" s="78"/>
@@ -19022,21 +19051,21 @@
       </c>
     </row>
     <row r="29" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B29" s="128" t="s">
+      <c r="B29" s="126" t="s">
         <v>278</v>
       </c>
-      <c r="C29" s="124" t="s">
+      <c r="C29" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="124"/>
-      <c r="E29" s="124"/>
-      <c r="F29" s="138" t="s">
+      <c r="D29" s="122"/>
+      <c r="E29" s="122"/>
+      <c r="F29" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G29" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H29" s="146">
+      <c r="H29" s="144">
         <v>22.05</v>
       </c>
       <c r="I29" s="70">
@@ -19045,10 +19074,10 @@
       <c r="J29" s="70">
         <v>1</v>
       </c>
-      <c r="K29" s="148" t="s">
+      <c r="K29" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="L29" s="145" t="s">
+      <c r="L29" s="143" t="s">
         <v>285</v>
       </c>
       <c r="M29" s="78"/>
@@ -19057,21 +19086,21 @@
       </c>
     </row>
     <row r="30" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B30" s="128" t="s">
+      <c r="B30" s="126" t="s">
         <v>279</v>
       </c>
-      <c r="C30" s="124" t="s">
+      <c r="C30" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="124"/>
-      <c r="E30" s="124"/>
-      <c r="F30" s="138" t="s">
+      <c r="D30" s="122"/>
+      <c r="E30" s="122"/>
+      <c r="F30" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G30" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H30" s="146">
+      <c r="H30" s="144">
         <v>22.05</v>
       </c>
       <c r="I30" s="70">
@@ -19080,10 +19109,10 @@
       <c r="J30" s="70">
         <v>1</v>
       </c>
-      <c r="K30" s="148" t="s">
+      <c r="K30" s="146" t="s">
         <v>286</v>
       </c>
-      <c r="L30" s="145" t="s">
+      <c r="L30" s="143" t="s">
         <v>287</v>
       </c>
       <c r="M30" s="78"/>
@@ -19092,7 +19121,7 @@
       </c>
     </row>
     <row r="31" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B31" s="128" t="s">
+      <c r="B31" s="126" t="s">
         <v>280</v>
       </c>
       <c r="C31" s="15" t="s">
@@ -19100,13 +19129,13 @@
       </c>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
-      <c r="F31" s="138" t="s">
+      <c r="F31" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G31" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H31" s="146">
+      <c r="H31" s="144">
         <v>22.05</v>
       </c>
       <c r="I31" s="70">
@@ -19115,10 +19144,10 @@
       <c r="J31" s="70">
         <v>1</v>
       </c>
-      <c r="K31" s="148" t="s">
+      <c r="K31" s="146" t="s">
         <v>288</v>
       </c>
-      <c r="L31" s="145" t="s">
+      <c r="L31" s="143" t="s">
         <v>289</v>
       </c>
       <c r="M31" s="78"/>
@@ -19135,7 +19164,7 @@
       </c>
       <c r="D32" s="70"/>
       <c r="E32" s="70"/>
-      <c r="F32" s="138" t="s">
+      <c r="F32" s="136" t="s">
         <v>291</v>
       </c>
       <c r="G32" s="70" t="s">
@@ -19150,10 +19179,10 @@
       <c r="J32" s="70">
         <v>1</v>
       </c>
-      <c r="K32" s="140" t="s">
+      <c r="K32" s="138" t="s">
         <v>293</v>
       </c>
-      <c r="L32" s="142" t="s">
+      <c r="L32" s="140" t="s">
         <v>294</v>
       </c>
       <c r="M32" s="19"/>
@@ -19170,7 +19199,7 @@
       </c>
       <c r="D33" s="70"/>
       <c r="E33" s="70"/>
-      <c r="F33" s="138" t="s">
+      <c r="F33" s="136" t="s">
         <v>291</v>
       </c>
       <c r="G33" s="70" t="s">
@@ -19185,10 +19214,10 @@
       <c r="J33" s="70">
         <v>1</v>
       </c>
-      <c r="K33" s="140" t="s">
+      <c r="K33" s="138" t="s">
         <v>296</v>
       </c>
-      <c r="L33" s="142" t="s">
+      <c r="L33" s="140" t="s">
         <v>294</v>
       </c>
       <c r="M33" s="19"/>
@@ -19205,7 +19234,7 @@
       </c>
       <c r="D34" s="70"/>
       <c r="E34" s="70"/>
-      <c r="F34" s="138" t="s">
+      <c r="F34" s="136" t="s">
         <v>291</v>
       </c>
       <c r="G34" s="70" t="s">
@@ -19220,10 +19249,10 @@
       <c r="J34" s="70">
         <v>1</v>
       </c>
-      <c r="K34" s="140" t="s">
+      <c r="K34" s="138" t="s">
         <v>298</v>
       </c>
-      <c r="L34" s="142" t="s">
+      <c r="L34" s="140" t="s">
         <v>294</v>
       </c>
       <c r="M34" s="19"/>
@@ -19240,7 +19269,7 @@
       </c>
       <c r="D35" s="70"/>
       <c r="E35" s="70"/>
-      <c r="F35" s="138" t="s">
+      <c r="F35" s="136" t="s">
         <v>291</v>
       </c>
       <c r="G35" s="70" t="s">
@@ -19255,10 +19284,10 @@
       <c r="J35" s="70">
         <v>1</v>
       </c>
-      <c r="K35" s="140" t="s">
+      <c r="K35" s="138" t="s">
         <v>300</v>
       </c>
-      <c r="L35" s="142" t="s">
+      <c r="L35" s="140" t="s">
         <v>294</v>
       </c>
       <c r="M35" s="19"/>
@@ -19275,7 +19304,7 @@
       </c>
       <c r="D36" s="70"/>
       <c r="E36" s="70"/>
-      <c r="F36" s="138" t="s">
+      <c r="F36" s="136" t="s">
         <v>291</v>
       </c>
       <c r="G36" s="70" t="s">
@@ -19290,10 +19319,10 @@
       <c r="J36" s="70">
         <v>1</v>
       </c>
-      <c r="K36" s="140" t="s">
+      <c r="K36" s="138" t="s">
         <v>275</v>
       </c>
-      <c r="L36" s="142" t="s">
+      <c r="L36" s="140" t="s">
         <v>294</v>
       </c>
       <c r="M36" s="19"/>
@@ -19310,7 +19339,7 @@
       </c>
       <c r="D37" s="70"/>
       <c r="E37" s="70"/>
-      <c r="F37" s="138" t="s">
+      <c r="F37" s="136" t="s">
         <v>291</v>
       </c>
       <c r="G37" s="70" t="s">
@@ -19325,10 +19354,10 @@
       <c r="J37" s="70">
         <v>1</v>
       </c>
-      <c r="K37" s="140" t="s">
+      <c r="K37" s="138" t="s">
         <v>303</v>
       </c>
-      <c r="L37" s="142" t="s">
+      <c r="L37" s="140" t="s">
         <v>294</v>
       </c>
       <c r="M37" s="19"/>
@@ -19345,7 +19374,7 @@
       </c>
       <c r="D38" s="70"/>
       <c r="E38" s="70"/>
-      <c r="F38" s="138" t="s">
+      <c r="F38" s="136" t="s">
         <v>291</v>
       </c>
       <c r="G38" s="70" t="s">
@@ -19360,10 +19389,10 @@
       <c r="J38" s="70">
         <v>1</v>
       </c>
-      <c r="K38" s="140" t="s">
+      <c r="K38" s="138" t="s">
         <v>305</v>
       </c>
-      <c r="L38" s="142" t="s">
+      <c r="L38" s="140" t="s">
         <v>294</v>
       </c>
       <c r="M38" s="19"/>
@@ -19380,7 +19409,7 @@
       </c>
       <c r="D39" s="70"/>
       <c r="E39" s="70"/>
-      <c r="F39" s="138" t="s">
+      <c r="F39" s="136" t="s">
         <v>291</v>
       </c>
       <c r="G39" s="70" t="s">
@@ -19395,10 +19424,10 @@
       <c r="J39" s="70">
         <v>1</v>
       </c>
-      <c r="K39" s="140" t="s">
+      <c r="K39" s="138" t="s">
         <v>307</v>
       </c>
-      <c r="L39" s="142" t="s">
+      <c r="L39" s="140" t="s">
         <v>308</v>
       </c>
       <c r="N39" s="27" t="s">
@@ -19414,7 +19443,7 @@
       </c>
       <c r="D40" s="70"/>
       <c r="E40" s="70"/>
-      <c r="F40" s="138" t="s">
+      <c r="F40" s="136" t="s">
         <v>291</v>
       </c>
       <c r="G40" s="70" t="s">
@@ -19429,10 +19458,10 @@
       <c r="J40" s="70">
         <v>1</v>
       </c>
-      <c r="K40" s="140" t="s">
+      <c r="K40" s="138" t="s">
         <v>310</v>
       </c>
-      <c r="L40" s="142" t="s">
+      <c r="L40" s="140" t="s">
         <v>308</v>
       </c>
       <c r="N40" s="27" t="s">
@@ -19448,7 +19477,7 @@
       </c>
       <c r="D41" s="70"/>
       <c r="E41" s="70"/>
-      <c r="F41" s="138" t="s">
+      <c r="F41" s="136" t="s">
         <v>291</v>
       </c>
       <c r="G41" s="70" t="s">
@@ -19463,16 +19492,16 @@
       <c r="J41" s="70">
         <v>1</v>
       </c>
-      <c r="K41" s="140" t="s">
+      <c r="K41" s="138" t="s">
         <v>312</v>
       </c>
-      <c r="L41" s="142" t="s">
+      <c r="L41" s="140" t="s">
         <v>308</v>
       </c>
       <c r="N41" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="Q41" s="138"/>
+      <c r="Q41" s="136"/>
     </row>
     <row r="42" spans="2:17" ht="13.5" customHeight="1">
       <c r="B42" s="29" t="s">
@@ -19483,7 +19512,7 @@
       </c>
       <c r="D42" s="70"/>
       <c r="E42" s="70"/>
-      <c r="F42" s="149" t="s">
+      <c r="F42" s="147" t="s">
         <v>314</v>
       </c>
       <c r="G42" s="70" t="s">
@@ -19498,10 +19527,10 @@
       <c r="J42" s="70">
         <v>1</v>
       </c>
-      <c r="K42" s="140" t="s">
+      <c r="K42" s="138" t="s">
         <v>315</v>
       </c>
-      <c r="L42" s="142" t="s">
+      <c r="L42" s="140" t="s">
         <v>221</v>
       </c>
       <c r="N42" s="27" t="s">
@@ -19517,7 +19546,7 @@
       </c>
       <c r="D43" s="70"/>
       <c r="E43" s="70"/>
-      <c r="F43" s="149" t="s">
+      <c r="F43" s="147" t="s">
         <v>314</v>
       </c>
       <c r="G43" s="70" t="s">
@@ -19532,10 +19561,10 @@
       <c r="J43" s="70">
         <v>1</v>
       </c>
-      <c r="K43" s="140" t="s">
+      <c r="K43" s="138" t="s">
         <v>317</v>
       </c>
-      <c r="L43" s="142" t="s">
+      <c r="L43" s="140" t="s">
         <v>221</v>
       </c>
       <c r="N43" s="27" t="s">
@@ -19551,7 +19580,7 @@
       </c>
       <c r="D44" s="70"/>
       <c r="E44" s="70"/>
-      <c r="F44" s="138" t="s">
+      <c r="F44" s="136" t="s">
         <v>314</v>
       </c>
       <c r="G44" s="70" t="s">
@@ -19566,10 +19595,10 @@
       <c r="J44" s="70">
         <v>1</v>
       </c>
-      <c r="K44" s="140" t="s">
+      <c r="K44" s="138" t="s">
         <v>319</v>
       </c>
-      <c r="L44" s="142" t="s">
+      <c r="L44" s="140" t="s">
         <v>221</v>
       </c>
       <c r="N44" s="27" t="s">
@@ -19589,7 +19618,7 @@
       <c r="H45" s="70"/>
       <c r="I45" s="70"/>
       <c r="J45" s="70"/>
-      <c r="K45" s="140"/>
+      <c r="K45" s="138"/>
       <c r="L45" s="88"/>
       <c r="N45" s="27" t="s">
         <v>93</v>
@@ -19608,7 +19637,7 @@
       <c r="H46" s="70"/>
       <c r="I46" s="70"/>
       <c r="J46" s="70"/>
-      <c r="K46" s="140"/>
+      <c r="K46" s="138"/>
       <c r="L46" s="88"/>
       <c r="N46" s="27" t="s">
         <v>93</v>
@@ -19628,7 +19657,7 @@
       <c r="I47" s="70"/>
       <c r="J47" s="70"/>
       <c r="K47" s="70"/>
-      <c r="L47" s="142"/>
+      <c r="L47" s="140"/>
       <c r="N47" s="27" t="s">
         <v>93</v>
       </c>
@@ -19657,10 +19686,10 @@
       <c r="J48" s="70">
         <v>2</v>
       </c>
-      <c r="K48" s="140" t="s">
+      <c r="K48" s="138" t="s">
         <v>322</v>
       </c>
-      <c r="L48" s="142" t="s">
+      <c r="L48" s="140" t="s">
         <v>323</v>
       </c>
       <c r="N48" s="27" t="s">
@@ -19668,7 +19697,7 @@
       </c>
     </row>
     <row r="49" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B49" s="150" t="s">
+      <c r="B49" s="148" t="s">
         <v>178</v>
       </c>
       <c r="C49" s="70" t="s">
@@ -19676,7 +19705,7 @@
       </c>
       <c r="D49" s="70"/>
       <c r="E49" s="70"/>
-      <c r="F49" s="138" t="s">
+      <c r="F49" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G49" s="70" t="s">
@@ -19691,7 +19720,7 @@
       <c r="J49" s="70">
         <v>1</v>
       </c>
-      <c r="K49" s="140" t="s">
+      <c r="K49" s="138" t="s">
         <v>273</v>
       </c>
       <c r="L49" s="88" t="s">
@@ -19700,7 +19729,7 @@
       <c r="N49" s="27"/>
     </row>
     <row r="50" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B50" s="150" t="s">
+      <c r="B50" s="148" t="s">
         <v>179</v>
       </c>
       <c r="C50" s="70" t="s">
@@ -19723,7 +19752,7 @@
       <c r="J50" s="70">
         <v>1</v>
       </c>
-      <c r="K50" s="140" t="s">
+      <c r="K50" s="138" t="s">
         <v>324</v>
       </c>
       <c r="L50" s="88" t="s">
@@ -19755,10 +19784,10 @@
       <c r="J51" s="70">
         <v>1</v>
       </c>
-      <c r="K51" s="140" t="s">
+      <c r="K51" s="138" t="s">
         <v>265</v>
       </c>
-      <c r="L51" s="142" t="s">
+      <c r="L51" s="140" t="s">
         <v>326</v>
       </c>
       <c r="N51" s="27" t="s">
@@ -19774,7 +19803,7 @@
       </c>
       <c r="D52" s="70"/>
       <c r="E52" s="70"/>
-      <c r="F52" s="138" t="s">
+      <c r="F52" s="136" t="s">
         <v>195</v>
       </c>
       <c r="G52" s="70" t="s">
@@ -19789,10 +19818,10 @@
       <c r="J52" s="70">
         <v>1</v>
       </c>
-      <c r="K52" s="140" t="s">
+      <c r="K52" s="138" t="s">
         <v>263</v>
       </c>
-      <c r="L52" s="142" t="s">
+      <c r="L52" s="140" t="s">
         <v>328</v>
       </c>
       <c r="N52" s="27" t="s">
@@ -19823,10 +19852,10 @@
       <c r="J53" s="70">
         <v>1</v>
       </c>
-      <c r="K53" s="140" t="s">
+      <c r="K53" s="138" t="s">
         <v>330</v>
       </c>
-      <c r="L53" s="142" t="s">
+      <c r="L53" s="140" t="s">
         <v>331</v>
       </c>
       <c r="N53" s="27" t="s">
@@ -19857,10 +19886,10 @@
       <c r="J54" s="70">
         <v>1</v>
       </c>
-      <c r="K54" s="140" t="s">
+      <c r="K54" s="138" t="s">
         <v>333</v>
       </c>
-      <c r="L54" s="142" t="s">
+      <c r="L54" s="140" t="s">
         <v>334</v>
       </c>
       <c r="N54" s="27" t="s">
@@ -19891,10 +19920,10 @@
       <c r="J55" s="70">
         <v>1</v>
       </c>
-      <c r="K55" s="140" t="s">
+      <c r="K55" s="138" t="s">
         <v>336</v>
       </c>
-      <c r="L55" s="142" t="s">
+      <c r="L55" s="140" t="s">
         <v>337</v>
       </c>
       <c r="N55" s="27" t="s">
@@ -19925,10 +19954,10 @@
       <c r="J56" s="70">
         <v>1</v>
       </c>
-      <c r="K56" s="140" t="s">
+      <c r="K56" s="138" t="s">
         <v>273</v>
       </c>
-      <c r="L56" s="142" t="s">
+      <c r="L56" s="140" t="s">
         <v>339</v>
       </c>
       <c r="N56" s="27" t="s">
@@ -19942,14 +19971,14 @@
       <c r="C57" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="D57" s="124"/>
-      <c r="E57" s="124"/>
+      <c r="D57" s="122"/>
+      <c r="E57" s="122"/>
       <c r="G57" s="70"/>
       <c r="H57" s="70"/>
       <c r="I57" s="70"/>
       <c r="J57" s="70"/>
-      <c r="K57" s="140"/>
-      <c r="L57" s="142"/>
+      <c r="K57" s="138"/>
+      <c r="L57" s="140"/>
       <c r="N57" s="27" t="s">
         <v>93</v>
       </c>
@@ -19967,8 +19996,8 @@
       <c r="H58" s="70"/>
       <c r="I58" s="70"/>
       <c r="J58" s="70"/>
-      <c r="K58" s="140"/>
-      <c r="L58" s="142"/>
+      <c r="K58" s="138"/>
+      <c r="L58" s="140"/>
       <c r="M58" s="19"/>
       <c r="N58" s="27" t="s">
         <v>93</v>
@@ -19981,14 +20010,14 @@
       <c r="C59" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="D59" s="124"/>
-      <c r="E59" s="124"/>
+      <c r="D59" s="122"/>
+      <c r="E59" s="122"/>
       <c r="G59" s="70"/>
       <c r="H59" s="70"/>
       <c r="I59" s="70"/>
       <c r="J59" s="70"/>
-      <c r="K59" s="140"/>
-      <c r="L59" s="142"/>
+      <c r="K59" s="138"/>
+      <c r="L59" s="140"/>
       <c r="M59" s="19"/>
       <c r="N59" s="27" t="s">
         <v>93</v>
@@ -20001,14 +20030,14 @@
       <c r="C60" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="D60" s="124"/>
+      <c r="D60" s="122"/>
       <c r="E60" s="70"/>
       <c r="G60" s="70"/>
       <c r="H60" s="70"/>
       <c r="I60" s="70"/>
       <c r="J60" s="70"/>
-      <c r="K60" s="140"/>
-      <c r="L60" s="142"/>
+      <c r="K60" s="138"/>
+      <c r="L60" s="140"/>
       <c r="M60" s="19"/>
       <c r="N60" s="27" t="s">
         <v>93</v>
@@ -20038,10 +20067,10 @@
       <c r="J61" s="70">
         <v>1</v>
       </c>
-      <c r="K61" s="140" t="s">
+      <c r="K61" s="138" t="s">
         <v>341</v>
       </c>
-      <c r="L61" s="142" t="s">
+      <c r="L61" s="140" t="s">
         <v>342</v>
       </c>
       <c r="M61" s="19"/>
@@ -20073,10 +20102,10 @@
       <c r="J62" s="70">
         <v>1</v>
       </c>
-      <c r="K62" s="140" t="s">
+      <c r="K62" s="138" t="s">
         <v>344</v>
       </c>
-      <c r="L62" s="142" t="s">
+      <c r="L62" s="140" t="s">
         <v>345</v>
       </c>
       <c r="M62" s="19"/>
@@ -20108,10 +20137,10 @@
       <c r="J63" s="70">
         <v>1</v>
       </c>
-      <c r="K63" s="140" t="s">
+      <c r="K63" s="138" t="s">
         <v>347</v>
       </c>
-      <c r="L63" s="142" t="s">
+      <c r="L63" s="140" t="s">
         <v>348</v>
       </c>
       <c r="M63" s="19"/>
@@ -20128,7 +20157,7 @@
       </c>
       <c r="D64" s="83"/>
       <c r="E64" s="83"/>
-      <c r="F64" s="151" t="s">
+      <c r="F64" s="149" t="s">
         <v>350</v>
       </c>
       <c r="G64" s="83" t="s">
@@ -20143,10 +20172,10 @@
       <c r="J64" s="83">
         <v>1</v>
       </c>
-      <c r="K64" s="152" t="s">
+      <c r="K64" s="150" t="s">
         <v>351</v>
       </c>
-      <c r="L64" s="153" t="s">
+      <c r="L64" s="151" t="s">
         <v>352</v>
       </c>
       <c r="M64" s="19"/>
@@ -20155,7 +20184,7 @@
       </c>
     </row>
     <row r="65" spans="2:13" ht="13.5" customHeight="1">
-      <c r="B65" s="154"/>
+      <c r="B65" s="152"/>
       <c r="C65" s="19">
         <f>COUNTA(C37:C64)</f>
         <v>28</v>
@@ -25111,7 +25140,7 @@
       <c r="L3" s="11"/>
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B4" s="129" t="s">
+      <c r="B4" s="127" t="s">
         <v>177</v>
       </c>
       <c r="C4" s="14"/>
@@ -25122,8 +25151,8 @@
       <c r="H4" s="38"/>
       <c r="I4" s="38"/>
       <c r="J4" s="38"/>
-      <c r="K4" s="100"/>
-      <c r="L4" s="101"/>
+      <c r="K4" s="98"/>
+      <c r="L4" s="99"/>
       <c r="N4" s="19" t="s">
         <v>21</v>
       </c>
@@ -25138,7 +25167,7 @@
       </c>
       <c r="E5" s="24"/>
       <c r="F5" s="24"/>
-      <c r="L5" s="101"/>
+      <c r="L5" s="99"/>
       <c r="N5" s="27" t="s">
         <v>24</v>
       </c>
@@ -25157,8 +25186,8 @@
       <c r="H6" s="36"/>
       <c r="I6" s="36"/>
       <c r="J6" s="36"/>
-      <c r="K6" s="102"/>
-      <c r="L6" s="101"/>
+      <c r="K6" s="100"/>
+      <c r="L6" s="99"/>
       <c r="N6" s="27" t="s">
         <v>24</v>
       </c>
@@ -25172,13 +25201,13 @@
         <v>11</v>
       </c>
       <c r="E7" s="14"/>
-      <c r="F7" s="103"/>
-      <c r="G7" s="104"/>
-      <c r="H7" s="105"/>
-      <c r="I7" s="106"/>
-      <c r="J7" s="106"/>
-      <c r="K7" s="107"/>
-      <c r="L7" s="101"/>
+      <c r="F7" s="101"/>
+      <c r="G7" s="102"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="104"/>
+      <c r="J7" s="104"/>
+      <c r="K7" s="105"/>
+      <c r="L7" s="99"/>
       <c r="N7" s="27" t="s">
         <v>24</v>
       </c>
@@ -25192,13 +25221,13 @@
         <v>11</v>
       </c>
       <c r="E8" s="14"/>
-      <c r="F8" s="108"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="109"/>
-      <c r="J8" s="109"/>
-      <c r="K8" s="110"/>
-      <c r="L8" s="111"/>
+      <c r="F8" s="106"/>
+      <c r="G8" s="107"/>
+      <c r="H8" s="107"/>
+      <c r="I8" s="107"/>
+      <c r="J8" s="107"/>
+      <c r="K8" s="108"/>
+      <c r="L8" s="109"/>
       <c r="N8" s="27" t="s">
         <v>93</v>
       </c>
@@ -25212,13 +25241,13 @@
         <v>11</v>
       </c>
       <c r="E9" s="68"/>
-      <c r="F9" s="112"/>
-      <c r="G9" s="113"/>
-      <c r="H9" s="113"/>
-      <c r="I9" s="113"/>
-      <c r="J9" s="113"/>
-      <c r="K9" s="114"/>
-      <c r="L9" s="115"/>
+      <c r="F9" s="110"/>
+      <c r="G9" s="111"/>
+      <c r="H9" s="111"/>
+      <c r="I9" s="111"/>
+      <c r="J9" s="111"/>
+      <c r="K9" s="112"/>
+      <c r="L9" s="113"/>
       <c r="M9" s="78"/>
       <c r="N9" s="27" t="s">
         <v>24</v>
@@ -25233,13 +25262,13 @@
         <v>11</v>
       </c>
       <c r="E10" s="68"/>
-      <c r="F10" s="112"/>
-      <c r="G10" s="113"/>
-      <c r="H10" s="113"/>
-      <c r="I10" s="113"/>
-      <c r="J10" s="113"/>
-      <c r="K10" s="114"/>
-      <c r="L10" s="115"/>
+      <c r="F10" s="110"/>
+      <c r="G10" s="111"/>
+      <c r="H10" s="111"/>
+      <c r="I10" s="111"/>
+      <c r="J10" s="111"/>
+      <c r="K10" s="112"/>
+      <c r="L10" s="113"/>
       <c r="M10" s="78"/>
       <c r="N10" s="27" t="s">
         <v>24</v>
@@ -25254,13 +25283,13 @@
         <v>11</v>
       </c>
       <c r="E11" s="68"/>
-      <c r="F11" s="116"/>
-      <c r="G11" s="104"/>
-      <c r="H11" s="104"/>
-      <c r="I11" s="104"/>
-      <c r="J11" s="104"/>
-      <c r="K11" s="117"/>
-      <c r="L11" s="118"/>
+      <c r="F11" s="114"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="102"/>
+      <c r="I11" s="102"/>
+      <c r="J11" s="102"/>
+      <c r="K11" s="115"/>
+      <c r="L11" s="116"/>
       <c r="M11" s="78"/>
       <c r="N11" s="27" t="s">
         <v>24</v>
@@ -25275,13 +25304,13 @@
         <v>11</v>
       </c>
       <c r="E12" s="24"/>
-      <c r="F12" s="119"/>
-      <c r="G12" s="120"/>
-      <c r="H12" s="120"/>
-      <c r="I12" s="120"/>
-      <c r="J12" s="120"/>
-      <c r="K12" s="117"/>
-      <c r="L12" s="118"/>
+      <c r="F12" s="117"/>
+      <c r="G12" s="118"/>
+      <c r="H12" s="118"/>
+      <c r="I12" s="118"/>
+      <c r="J12" s="118"/>
+      <c r="K12" s="115"/>
+      <c r="L12" s="116"/>
       <c r="N12" s="27" t="s">
         <v>24</v>
       </c>
@@ -25298,12 +25327,12 @@
       <c r="F13" s="60" t="s">
         <v>159</v>
       </c>
-      <c r="G13" s="120"/>
-      <c r="H13" s="120"/>
-      <c r="I13" s="120"/>
-      <c r="J13" s="120"/>
-      <c r="K13" s="120"/>
-      <c r="L13" s="118"/>
+      <c r="G13" s="118"/>
+      <c r="H13" s="118"/>
+      <c r="I13" s="118"/>
+      <c r="J13" s="118"/>
+      <c r="K13" s="118"/>
+      <c r="L13" s="116"/>
       <c r="N13" s="27" t="s">
         <v>93</v>
       </c>
@@ -25320,12 +25349,12 @@
       <c r="F14" s="60" t="s">
         <v>161</v>
       </c>
-      <c r="G14" s="104"/>
-      <c r="H14" s="105"/>
-      <c r="I14" s="106"/>
-      <c r="J14" s="106"/>
-      <c r="K14" s="107"/>
-      <c r="L14" s="118"/>
+      <c r="G14" s="102"/>
+      <c r="H14" s="103"/>
+      <c r="I14" s="104"/>
+      <c r="J14" s="104"/>
+      <c r="K14" s="105"/>
+      <c r="L14" s="116"/>
       <c r="N14" s="27" t="s">
         <v>93</v>
       </c>
@@ -25342,12 +25371,12 @@
       <c r="F15" s="60" t="s">
         <v>163</v>
       </c>
-      <c r="G15" s="120"/>
-      <c r="H15" s="120"/>
-      <c r="I15" s="120"/>
-      <c r="J15" s="120"/>
-      <c r="K15" s="120"/>
-      <c r="L15" s="118"/>
+      <c r="G15" s="118"/>
+      <c r="H15" s="118"/>
+      <c r="I15" s="118"/>
+      <c r="J15" s="118"/>
+      <c r="K15" s="118"/>
+      <c r="L15" s="116"/>
       <c r="N15" s="27" t="s">
         <v>93</v>
       </c>
@@ -25361,13 +25390,13 @@
         <v>11</v>
       </c>
       <c r="E16" s="24"/>
-      <c r="F16" s="119"/>
-      <c r="G16" s="120"/>
-      <c r="H16" s="120"/>
-      <c r="I16" s="120"/>
-      <c r="J16" s="120"/>
-      <c r="K16" s="120"/>
-      <c r="L16" s="115"/>
+      <c r="F16" s="117"/>
+      <c r="G16" s="118"/>
+      <c r="H16" s="118"/>
+      <c r="I16" s="118"/>
+      <c r="J16" s="118"/>
+      <c r="K16" s="118"/>
+      <c r="L16" s="113"/>
       <c r="N16" s="27" t="s">
         <v>93</v>
       </c>
@@ -25381,13 +25410,13 @@
         <v>11</v>
       </c>
       <c r="E17" s="24"/>
-      <c r="F17" s="119"/>
-      <c r="G17" s="120"/>
-      <c r="H17" s="120"/>
-      <c r="I17" s="120"/>
-      <c r="J17" s="120"/>
-      <c r="K17" s="120"/>
-      <c r="L17" s="118"/>
+      <c r="F17" s="117"/>
+      <c r="G17" s="118"/>
+      <c r="H17" s="118"/>
+      <c r="I17" s="118"/>
+      <c r="J17" s="118"/>
+      <c r="K17" s="118"/>
+      <c r="L17" s="116"/>
       <c r="N17" s="27" t="s">
         <v>93</v>
       </c>
@@ -25401,13 +25430,13 @@
         <v>11</v>
       </c>
       <c r="E18" s="24"/>
-      <c r="F18" s="119"/>
-      <c r="G18" s="120"/>
-      <c r="H18" s="120"/>
-      <c r="I18" s="120"/>
-      <c r="J18" s="120"/>
-      <c r="K18" s="120"/>
-      <c r="L18" s="118"/>
+      <c r="F18" s="117"/>
+      <c r="G18" s="118"/>
+      <c r="H18" s="118"/>
+      <c r="I18" s="118"/>
+      <c r="J18" s="118"/>
+      <c r="K18" s="118"/>
+      <c r="L18" s="116"/>
       <c r="N18" s="27" t="s">
         <v>24</v>
       </c>
@@ -25427,7 +25456,7 @@
       <c r="I19" s="71"/>
       <c r="J19" s="71"/>
       <c r="K19" s="71"/>
-      <c r="L19" s="118"/>
+      <c r="L19" s="116"/>
       <c r="N19" s="27" t="s">
         <v>24</v>
       </c>
@@ -25446,8 +25475,8 @@
       <c r="H20" s="78"/>
       <c r="I20" s="78"/>
       <c r="J20" s="78"/>
-      <c r="K20" s="121"/>
-      <c r="L20" s="118"/>
+      <c r="K20" s="119"/>
+      <c r="L20" s="116"/>
       <c r="N20" s="27" t="s">
         <v>131</v>
       </c>
@@ -25467,7 +25496,7 @@
       <c r="I21" s="71"/>
       <c r="J21" s="71"/>
       <c r="K21" s="71"/>
-      <c r="L21" s="118"/>
+      <c r="L21" s="116"/>
       <c r="N21" s="27" t="s">
         <v>93</v>
       </c>
@@ -25481,7 +25510,7 @@
         <v>11</v>
       </c>
       <c r="E22" s="14"/>
-      <c r="F22" s="122" t="s">
+      <c r="F22" s="120" t="s">
         <v>171</v>
       </c>
       <c r="G22" s="71"/>
@@ -25489,7 +25518,7 @@
       <c r="I22" s="71"/>
       <c r="J22" s="71"/>
       <c r="K22" s="71"/>
-      <c r="L22" s="118"/>
+      <c r="L22" s="116"/>
       <c r="N22" s="27" t="s">
         <v>93</v>
       </c>
@@ -25509,7 +25538,7 @@
       <c r="I23" s="71"/>
       <c r="J23" s="71"/>
       <c r="K23" s="71"/>
-      <c r="L23" s="118"/>
+      <c r="L23" s="116"/>
       <c r="N23" s="27" t="s">
         <v>24</v>
       </c>
@@ -25529,7 +25558,7 @@
       <c r="I24" s="71"/>
       <c r="J24" s="71"/>
       <c r="K24" s="71"/>
-      <c r="L24" s="115"/>
+      <c r="L24" s="113"/>
       <c r="N24" s="27" t="s">
         <v>93</v>
       </c>
@@ -25544,7 +25573,7 @@
       </c>
       <c r="E25" s="14"/>
       <c r="F25" s="24"/>
-      <c r="L25" s="118"/>
+      <c r="L25" s="116"/>
       <c r="N25" s="27" t="s">
         <v>24</v>
       </c>
@@ -25559,19 +25588,19 @@
       </c>
       <c r="E26" s="80"/>
       <c r="F26" s="80"/>
-      <c r="G26" s="123"/>
-      <c r="H26" s="123"/>
-      <c r="I26" s="123"/>
-      <c r="J26" s="123"/>
-      <c r="K26" s="125"/>
-      <c r="L26" s="126"/>
+      <c r="G26" s="121"/>
+      <c r="H26" s="121"/>
+      <c r="I26" s="121"/>
+      <c r="J26" s="121"/>
+      <c r="K26" s="123"/>
+      <c r="L26" s="124"/>
       <c r="M26" s="78"/>
       <c r="N26" s="27" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B27" s="99"/>
+      <c r="B27" s="97"/>
       <c r="C27" s="78">
         <f t="shared" ref="C27:E27" si="0">COUNTA(C4:C26)</f>
         <v>1</v>
@@ -25594,7 +25623,7 @@
       <c r="M27" s="78"/>
     </row>
     <row r="28" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B28" s="99"/>
+      <c r="B28" s="97"/>
       <c r="C28" s="38"/>
       <c r="D28" s="38"/>
       <c r="E28" s="38"/>
@@ -30547,19 +30576,19 @@
       <c r="L3" s="11"/>
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B4" s="129" t="s">
+      <c r="B4" s="127" t="s">
         <v>177</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="14"/>
-      <c r="E4" s="124"/>
-      <c r="F4" s="124"/>
-      <c r="G4" s="124"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="122"/>
+      <c r="G4" s="122"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
-      <c r="K4" s="132"/>
-      <c r="L4" s="135"/>
+      <c r="K4" s="130"/>
+      <c r="L4" s="133"/>
     </row>
     <row r="5" spans="1:26" ht="13.5" customHeight="1">
       <c r="B5" s="13" t="s">
@@ -30570,16 +30599,16 @@
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
-      <c r="F5" s="138"/>
+      <c r="F5" s="136"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
-      <c r="K5" s="132"/>
-      <c r="L5" s="135"/>
+      <c r="K5" s="130"/>
+      <c r="L5" s="133"/>
     </row>
     <row r="6" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B6" s="130" t="s">
+      <c r="B6" s="128" t="s">
         <v>181</v>
       </c>
       <c r="C6" s="15" t="s">
@@ -30587,10 +30616,10 @@
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="138" t="s">
+      <c r="F6" s="136" t="s">
         <v>215</v>
       </c>
-      <c r="G6" s="131" t="s">
+      <c r="G6" s="129" t="s">
         <v>18</v>
       </c>
       <c r="H6" s="14">
@@ -30602,15 +30631,15 @@
       <c r="J6" s="14">
         <v>1</v>
       </c>
-      <c r="K6" s="134" t="s">
+      <c r="K6" s="132" t="s">
         <v>180</v>
       </c>
-      <c r="L6" s="136" t="s">
+      <c r="L6" s="134" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B7" s="130" t="s">
+      <c r="B7" s="128" t="s">
         <v>184</v>
       </c>
       <c r="C7" s="15" t="s">
@@ -30618,30 +30647,30 @@
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
-      <c r="F7" s="138" t="s">
+      <c r="F7" s="136" t="s">
         <v>215</v>
       </c>
-      <c r="G7" s="131" t="s">
+      <c r="G7" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="124">
+      <c r="H7" s="122">
         <v>16</v>
       </c>
-      <c r="I7" s="124">
+      <c r="I7" s="122">
         <v>32</v>
       </c>
       <c r="J7" s="14">
         <v>1</v>
       </c>
-      <c r="K7" s="134" t="s">
+      <c r="K7" s="132" t="s">
         <v>182</v>
       </c>
-      <c r="L7" s="136" t="s">
+      <c r="L7" s="134" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B8" s="130" t="s">
+      <c r="B8" s="128" t="s">
         <v>185</v>
       </c>
       <c r="C8" s="15" t="s">
@@ -30649,30 +30678,30 @@
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
-      <c r="F8" s="138" t="s">
+      <c r="F8" s="136" t="s">
         <v>215</v>
       </c>
-      <c r="G8" s="131" t="s">
+      <c r="G8" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="124">
+      <c r="H8" s="122">
         <v>16</v>
       </c>
-      <c r="I8" s="124">
+      <c r="I8" s="122">
         <v>32</v>
       </c>
-      <c r="J8" s="124">
+      <c r="J8" s="122">
         <v>1</v>
       </c>
-      <c r="K8" s="134" t="s">
+      <c r="K8" s="132" t="s">
         <v>183</v>
       </c>
-      <c r="L8" s="136" t="s">
+      <c r="L8" s="134" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B9" s="130" t="s">
+      <c r="B9" s="128" t="s">
         <v>186</v>
       </c>
       <c r="C9" s="25" t="s">
@@ -30680,30 +30709,30 @@
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
-      <c r="F9" s="138" t="s">
+      <c r="F9" s="136" t="s">
         <v>215</v>
       </c>
-      <c r="G9" s="131" t="s">
+      <c r="G9" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="124">
+      <c r="H9" s="122">
         <v>16</v>
       </c>
-      <c r="I9" s="124">
+      <c r="I9" s="122">
         <v>32</v>
       </c>
-      <c r="J9" s="124">
+      <c r="J9" s="122">
         <v>1</v>
       </c>
-      <c r="K9" s="134" t="s">
+      <c r="K9" s="132" t="s">
         <v>197</v>
       </c>
-      <c r="L9" s="136" t="s">
+      <c r="L9" s="134" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B10" s="130" t="s">
+      <c r="B10" s="128" t="s">
         <v>188</v>
       </c>
       <c r="C10" s="15" t="s">
@@ -30711,30 +30740,30 @@
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
-      <c r="F10" s="138" t="s">
+      <c r="F10" s="136" t="s">
         <v>217</v>
       </c>
-      <c r="G10" s="131" t="s">
+      <c r="G10" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="124">
+      <c r="H10" s="122">
         <v>16</v>
       </c>
-      <c r="I10" s="124">
+      <c r="I10" s="122">
         <v>32</v>
       </c>
-      <c r="J10" s="124">
+      <c r="J10" s="122">
         <v>1</v>
       </c>
-      <c r="K10" s="134" t="s">
+      <c r="K10" s="132" t="s">
         <v>187</v>
       </c>
-      <c r="L10" s="136" t="s">
+      <c r="L10" s="134" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B11" s="130" t="s">
+      <c r="B11" s="128" t="s">
         <v>190</v>
       </c>
       <c r="C11" s="15" t="s">
@@ -30742,30 +30771,30 @@
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
-      <c r="F11" s="138" t="s">
+      <c r="F11" s="136" t="s">
         <v>217</v>
       </c>
-      <c r="G11" s="131" t="s">
+      <c r="G11" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="124">
+      <c r="H11" s="122">
         <v>16</v>
       </c>
-      <c r="I11" s="124">
+      <c r="I11" s="122">
         <v>32</v>
       </c>
-      <c r="J11" s="124">
+      <c r="J11" s="122">
         <v>1</v>
       </c>
-      <c r="K11" s="134" t="s">
+      <c r="K11" s="132" t="s">
         <v>189</v>
       </c>
-      <c r="L11" s="136" t="s">
+      <c r="L11" s="134" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B12" s="130" t="s">
+      <c r="B12" s="128" t="s">
         <v>192</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -30773,30 +30802,30 @@
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
-      <c r="F12" s="138" t="s">
+      <c r="F12" s="136" t="s">
         <v>217</v>
       </c>
-      <c r="G12" s="131" t="s">
+      <c r="G12" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="124">
+      <c r="H12" s="122">
         <v>16</v>
       </c>
-      <c r="I12" s="124">
+      <c r="I12" s="122">
         <v>32</v>
       </c>
-      <c r="J12" s="124">
+      <c r="J12" s="122">
         <v>1</v>
       </c>
-      <c r="K12" s="134" t="s">
+      <c r="K12" s="132" t="s">
         <v>191</v>
       </c>
-      <c r="L12" s="136" t="s">
+      <c r="L12" s="134" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B13" s="130" t="s">
+      <c r="B13" s="128" t="s">
         <v>194</v>
       </c>
       <c r="C13" s="25" t="s">
@@ -30804,30 +30833,30 @@
       </c>
       <c r="D13" s="24"/>
       <c r="E13" s="24"/>
-      <c r="F13" s="138" t="s">
+      <c r="F13" s="136" t="s">
         <v>218</v>
       </c>
-      <c r="G13" s="131" t="s">
+      <c r="G13" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="124">
+      <c r="H13" s="122">
         <v>16</v>
       </c>
-      <c r="I13" s="124">
+      <c r="I13" s="122">
         <v>32</v>
       </c>
-      <c r="J13" s="124">
+      <c r="J13" s="122">
         <v>1</v>
       </c>
-      <c r="K13" s="134" t="s">
+      <c r="K13" s="132" t="s">
         <v>193</v>
       </c>
-      <c r="L13" s="136" t="s">
+      <c r="L13" s="134" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B14" s="130" t="s">
+      <c r="B14" s="128" t="s">
         <v>199</v>
       </c>
       <c r="C14" s="63" t="s">
@@ -30835,95 +30864,95 @@
       </c>
       <c r="D14" s="68"/>
       <c r="E14" s="68"/>
-      <c r="F14" s="138" t="s">
+      <c r="F14" s="136" t="s">
         <v>219</v>
       </c>
-      <c r="G14" s="131" t="s">
+      <c r="G14" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="124">
+      <c r="H14" s="122">
         <v>16</v>
       </c>
-      <c r="I14" s="124">
+      <c r="I14" s="122">
         <v>32</v>
       </c>
-      <c r="J14" s="124">
+      <c r="J14" s="122">
         <v>1</v>
       </c>
-      <c r="K14" s="134" t="s">
+      <c r="K14" s="132" t="s">
         <v>198</v>
       </c>
-      <c r="L14" s="136" t="s">
+      <c r="L14" s="134" t="s">
         <v>220</v>
       </c>
       <c r="M14" s="78"/>
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B15" s="130" t="s">
+      <c r="B15" s="128" t="s">
         <v>201</v>
       </c>
-      <c r="C15" s="124" t="s">
+      <c r="C15" s="122" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="68"/>
       <c r="E15" s="68"/>
-      <c r="F15" s="138" t="s">
+      <c r="F15" s="136" t="s">
         <v>219</v>
       </c>
-      <c r="G15" s="131" t="s">
+      <c r="G15" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="124">
+      <c r="H15" s="122">
         <v>16</v>
       </c>
-      <c r="I15" s="124">
+      <c r="I15" s="122">
         <v>32</v>
       </c>
-      <c r="J15" s="124">
+      <c r="J15" s="122">
         <v>1</v>
       </c>
-      <c r="K15" s="134" t="s">
+      <c r="K15" s="132" t="s">
         <v>200</v>
       </c>
-      <c r="L15" s="136" t="s">
+      <c r="L15" s="134" t="s">
         <v>220</v>
       </c>
       <c r="M15" s="78"/>
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1">
-      <c r="B16" s="130" t="s">
+      <c r="B16" s="128" t="s">
         <v>203</v>
       </c>
-      <c r="C16" s="124" t="s">
+      <c r="C16" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="137"/>
+      <c r="D16" s="135"/>
       <c r="E16" s="68"/>
-      <c r="F16" s="138" t="s">
+      <c r="F16" s="136" t="s">
         <v>219</v>
       </c>
-      <c r="G16" s="131" t="s">
+      <c r="G16" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="124">
+      <c r="H16" s="122">
         <v>16</v>
       </c>
-      <c r="I16" s="124">
+      <c r="I16" s="122">
         <v>32</v>
       </c>
-      <c r="J16" s="124">
+      <c r="J16" s="122">
         <v>1</v>
       </c>
-      <c r="K16" s="134" t="s">
+      <c r="K16" s="132" t="s">
         <v>202</v>
       </c>
-      <c r="L16" s="136" t="s">
+      <c r="L16" s="134" t="s">
         <v>220</v>
       </c>
       <c r="M16" s="78"/>
     </row>
     <row r="17" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B17" s="130" t="s">
+      <c r="B17" s="128" t="s">
         <v>205</v>
       </c>
       <c r="C17" s="68" t="s">
@@ -30931,128 +30960,128 @@
       </c>
       <c r="D17" s="68"/>
       <c r="E17" s="68"/>
-      <c r="F17" s="138" t="s">
+      <c r="F17" s="136" t="s">
         <v>219</v>
       </c>
-      <c r="G17" s="131" t="s">
+      <c r="G17" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="124">
+      <c r="H17" s="122">
         <v>16</v>
       </c>
-      <c r="I17" s="124">
+      <c r="I17" s="122">
         <v>32</v>
       </c>
-      <c r="J17" s="124">
+      <c r="J17" s="122">
         <v>1</v>
       </c>
-      <c r="K17" s="134" t="s">
+      <c r="K17" s="132" t="s">
         <v>204</v>
       </c>
-      <c r="L17" s="136" t="s">
+      <c r="L17" s="134" t="s">
         <v>220</v>
       </c>
       <c r="M17" s="78"/>
     </row>
     <row r="18" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B18" s="130" t="s">
+      <c r="B18" s="128" t="s">
         <v>207</v>
       </c>
-      <c r="C18" s="124" t="s">
+      <c r="C18" s="122" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="68"/>
       <c r="E18" s="68"/>
-      <c r="F18" s="138" t="s">
+      <c r="F18" s="136" t="s">
         <v>222</v>
       </c>
-      <c r="G18" s="131" t="s">
+      <c r="G18" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="124">
+      <c r="H18" s="122">
         <v>16</v>
       </c>
-      <c r="I18" s="124">
+      <c r="I18" s="122">
         <v>32</v>
       </c>
-      <c r="J18" s="124">
+      <c r="J18" s="122">
         <v>1</v>
       </c>
-      <c r="K18" s="134" t="s">
+      <c r="K18" s="132" t="s">
         <v>206</v>
       </c>
-      <c r="L18" s="136" t="s">
+      <c r="L18" s="134" t="s">
         <v>221</v>
       </c>
       <c r="M18" s="78"/>
-      <c r="N18" s="138"/>
+      <c r="N18" s="136"/>
     </row>
     <row r="19" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B19" s="130" t="s">
+      <c r="B19" s="128" t="s">
         <v>209</v>
       </c>
-      <c r="C19" s="124" t="s">
+      <c r="C19" s="122" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="68"/>
       <c r="E19" s="68"/>
-      <c r="F19" s="138" t="s">
+      <c r="F19" s="136" t="s">
         <v>222</v>
       </c>
-      <c r="G19" s="131" t="s">
+      <c r="G19" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="124">
+      <c r="H19" s="122">
         <v>16</v>
       </c>
-      <c r="I19" s="124">
+      <c r="I19" s="122">
         <v>32</v>
       </c>
-      <c r="J19" s="124">
+      <c r="J19" s="122">
         <v>1</v>
       </c>
-      <c r="K19" s="134" t="s">
+      <c r="K19" s="132" t="s">
         <v>208</v>
       </c>
-      <c r="L19" s="136" t="s">
+      <c r="L19" s="134" t="s">
         <v>221</v>
       </c>
       <c r="M19" s="78"/>
     </row>
     <row r="20" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B20" s="130" t="s">
+      <c r="B20" s="128" t="s">
         <v>213</v>
       </c>
-      <c r="C20" s="124" t="s">
+      <c r="C20" s="122" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="68"/>
       <c r="E20" s="68"/>
-      <c r="F20" s="138" t="s">
+      <c r="F20" s="136" t="s">
         <v>222</v>
       </c>
-      <c r="G20" s="131" t="s">
+      <c r="G20" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="124">
+      <c r="H20" s="122">
         <v>16</v>
       </c>
-      <c r="I20" s="124">
+      <c r="I20" s="122">
         <v>32</v>
       </c>
-      <c r="J20" s="124">
+      <c r="J20" s="122">
         <v>1</v>
       </c>
-      <c r="K20" s="134" t="s">
+      <c r="K20" s="132" t="s">
         <v>210</v>
       </c>
-      <c r="L20" s="136" t="s">
+      <c r="L20" s="134" t="s">
         <v>221</v>
       </c>
       <c r="M20" s="78"/>
     </row>
     <row r="21" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B21" s="130" t="s">
+      <c r="B21" s="128" t="s">
         <v>212</v>
       </c>
       <c r="C21" s="68" t="s">
@@ -31060,25 +31089,25 @@
       </c>
       <c r="D21" s="68"/>
       <c r="E21" s="68"/>
-      <c r="F21" s="138" t="s">
+      <c r="F21" s="136" t="s">
         <v>222</v>
       </c>
-      <c r="G21" s="131" t="s">
+      <c r="G21" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="H21" s="124">
+      <c r="H21" s="122">
         <v>16</v>
       </c>
-      <c r="I21" s="124">
+      <c r="I21" s="122">
         <v>32</v>
       </c>
-      <c r="J21" s="124">
+      <c r="J21" s="122">
         <v>1</v>
       </c>
-      <c r="K21" s="134" t="s">
+      <c r="K21" s="132" t="s">
         <v>211</v>
       </c>
-      <c r="L21" s="136" t="s">
+      <c r="L21" s="134" t="s">
         <v>221</v>
       </c>
       <c r="M21" s="78"/>
@@ -31087,7 +31116,7 @@
       <c r="B22" s="79" t="s">
         <v>176</v>
       </c>
-      <c r="C22" s="127" t="s">
+      <c r="C22" s="125" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="80"/>
@@ -31097,8 +31126,8 @@
       <c r="H22" s="80"/>
       <c r="I22" s="80"/>
       <c r="J22" s="80"/>
-      <c r="K22" s="133"/>
-      <c r="L22" s="126"/>
+      <c r="K22" s="131"/>
+      <c r="L22" s="124"/>
       <c r="M22" s="78"/>
     </row>
     <row r="23" spans="2:14" ht="13.5" customHeight="1">
@@ -31110,7 +31139,7 @@
       <c r="C24" s="38"/>
       <c r="D24" s="38"/>
       <c r="E24" s="38"/>
-      <c r="F24" s="139"/>
+      <c r="F24" s="137"/>
     </row>
     <row r="25" spans="2:14" ht="13.5" customHeight="1">
       <c r="C25" s="38"/>
@@ -31128,7 +31157,7 @@
       <c r="E27" s="38"/>
     </row>
     <row r="28" spans="2:14" ht="13.5" customHeight="1">
-      <c r="F28" s="138"/>
+      <c r="F28" s="136"/>
     </row>
     <row r="29" spans="2:14" ht="13.5" customHeight="1">
       <c r="C29" s="38"/>

</xml_diff>

<commit_message>
Ordenado en carpetas y creado algún evento más
</commit_message>
<xml_diff>
--- a/Tablas de sonido/Tabla_metadatos_no_lineal.xlsx
+++ b/Tablas de sonido/Tabla_metadatos_no_lineal.xlsx
@@ -1556,7 +1556,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1961,6 +1961,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3484,7 +3487,7 @@
   <dimension ref="A1:Z1003"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3852,7 +3855,7 @@
       <c r="E13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="153" t="s">
         <v>33</v>
       </c>
       <c r="G13" s="15" t="s">
@@ -13262,7 +13265,7 @@
     <row r="26" spans="2:14" ht="13.5" customHeight="1">
       <c r="B26" s="97"/>
       <c r="C26" s="38">
-        <f t="shared" ref="C26:I26" si="0">COUNTA(C6:C25)</f>
+        <f t="shared" ref="C26:E26" si="0">COUNTA(C6:C25)</f>
         <v>0</v>
       </c>
       <c r="D26" s="38">

</xml_diff>